<commit_message>
erm i added previous data view but the data is like currently wrong rn my fault
</commit_message>
<xml_diff>
--- a/data/total_steam_titles.xlsx
+++ b/data/total_steam_titles.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenwang/Desktop/Makers/Roblox_Streamlit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenwang/Desktop/Makers/Steam_Roblox_Streamlit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E31589-AF96-AE4B-BDD5-A050C4B64E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9755F80-FA37-8046-9E9D-5285A94A9F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="1240" windowWidth="24960" windowHeight="16760" xr2:uid="{91033176-3A50-8A43-8B19-6289EA40BB69}"/>
   </bookViews>
   <sheets>
-    <sheet name="2024-07-18" sheetId="1" r:id="rId1"/>
-    <sheet name="2024-07-11" sheetId="2" r:id="rId2"/>
+    <sheet name="2024-07-23" sheetId="3" r:id="rId1"/>
+    <sheet name="2024-07-18" sheetId="1" r:id="rId2"/>
+    <sheet name="2024-07-11" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="550">
   <si>
     <t>Game</t>
   </si>
@@ -1679,6 +1680,15 @@
   </si>
   <si>
     <t>https://store.steampowered.com/app/1974050/Torchlight_Infinite?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>FromSoftware, Inc.</t>
+  </si>
+  <si>
+    <t>Battlefield‚Ñ¢ 2042 is a first-person shooter that marks the return to the iconic all-out warfare of the franchise.</t>
+  </si>
+  <si>
+    <t>Landfall</t>
   </si>
 </sst>
 </file>
@@ -2058,10 +2068,3806 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3978525E-3F5E-9048-BC93-38E6C42116E5}">
+  <dimension ref="A1:L101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>382</v>
+      </c>
+      <c r="D2" s="1">
+        <v>43090</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2">
+        <v>20525</v>
+      </c>
+      <c r="J2">
+        <v>2399234</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>346</v>
+      </c>
+      <c r="D3" s="1">
+        <v>41464</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3">
+        <v>20924</v>
+      </c>
+      <c r="J3">
+        <v>2280816</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>-2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45473</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4">
+        <v>67181</v>
+      </c>
+      <c r="K4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>-1</v>
+      </c>
+      <c r="C5">
+        <v>623</v>
+      </c>
+      <c r="D5" s="1">
+        <v>41142</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5">
+        <v>67944</v>
+      </c>
+      <c r="J5">
+        <v>8168969</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+      <c r="C6">
+        <v>125</v>
+      </c>
+      <c r="L6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7">
+        <v>-4</v>
+      </c>
+      <c r="C7">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44616</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>547</v>
+      </c>
+      <c r="G7" t="s">
+        <v>547</v>
+      </c>
+      <c r="H7" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I7">
+        <v>47657</v>
+      </c>
+      <c r="J7">
+        <v>681149</v>
+      </c>
+      <c r="K7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>193</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44139</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8">
+        <v>82284</v>
+      </c>
+      <c r="J8">
+        <v>918863</v>
+      </c>
+      <c r="K8" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45482</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9">
+        <v>50192</v>
+      </c>
+      <c r="K9" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10">
+        <v>-3</v>
+      </c>
+      <c r="C10">
+        <v>69</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45141</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I10">
+        <v>11130</v>
+      </c>
+      <c r="J10">
+        <v>562486</v>
+      </c>
+      <c r="K10" t="s">
+        <v>56</v>
+      </c>
+      <c r="L10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <v>-3</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>547</v>
+      </c>
+      <c r="G11" t="s">
+        <v>547</v>
+      </c>
+      <c r="H11" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="I11">
+        <v>36260</v>
+      </c>
+      <c r="J11">
+        <v>74979</v>
+      </c>
+      <c r="L11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <v>-2</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1">
+        <v>45462</v>
+      </c>
+      <c r="E12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="2">
+        <v>4.99</v>
+      </c>
+      <c r="I12">
+        <v>15391</v>
+      </c>
+      <c r="J12">
+        <v>18846</v>
+      </c>
+      <c r="K12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13">
+        <v>-4</v>
+      </c>
+      <c r="C13">
+        <v>153</v>
+      </c>
+      <c r="D13" s="1">
+        <v>44419</v>
+      </c>
+      <c r="E13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13">
+        <v>9201</v>
+      </c>
+      <c r="J13">
+        <v>238173</v>
+      </c>
+      <c r="K13" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14">
+        <v>-3</v>
+      </c>
+      <c r="C14">
+        <v>58</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44174</v>
+      </c>
+      <c r="E14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I14">
+        <v>8710</v>
+      </c>
+      <c r="J14">
+        <v>668206</v>
+      </c>
+      <c r="K14" t="s">
+        <v>74</v>
+      </c>
+      <c r="L14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1">
+        <v>43739</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15">
+        <v>4642</v>
+      </c>
+      <c r="J15">
+        <v>607354</v>
+      </c>
+      <c r="K15" t="s">
+        <v>78</v>
+      </c>
+      <c r="L15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16">
+        <v>-2</v>
+      </c>
+      <c r="C16">
+        <v>496</v>
+      </c>
+      <c r="D16" s="1">
+        <v>42108</v>
+      </c>
+      <c r="E16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="2">
+        <v>39.979999999999997</v>
+      </c>
+      <c r="I16">
+        <v>23641</v>
+      </c>
+      <c r="J16">
+        <v>1677214</v>
+      </c>
+      <c r="K16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1">
+        <v>45523</v>
+      </c>
+      <c r="E17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="K17" t="s">
+        <v>89</v>
+      </c>
+      <c r="L17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18">
+        <v>-5</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1">
+        <v>43804</v>
+      </c>
+      <c r="E18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I18">
+        <v>14648</v>
+      </c>
+      <c r="J18">
+        <v>550821</v>
+      </c>
+      <c r="K18" t="s">
+        <v>92</v>
+      </c>
+      <c r="L18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19">
+        <v>-2</v>
+      </c>
+      <c r="C19">
+        <v>241</v>
+      </c>
+      <c r="D19" s="1">
+        <v>41501</v>
+      </c>
+      <c r="E19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19">
+        <v>11615</v>
+      </c>
+      <c r="J19">
+        <v>512752</v>
+      </c>
+      <c r="K19" t="s">
+        <v>98</v>
+      </c>
+      <c r="L19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20">
+        <v>-8</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>44264</v>
+      </c>
+      <c r="E20" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" t="s">
+        <v>102</v>
+      </c>
+      <c r="G20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H20" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I20">
+        <v>17736</v>
+      </c>
+      <c r="J20">
+        <v>220264</v>
+      </c>
+      <c r="K20" t="s">
+        <v>104</v>
+      </c>
+      <c r="L20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21">
+        <v>-3</v>
+      </c>
+      <c r="C21">
+        <v>53</v>
+      </c>
+      <c r="D21" s="1">
+        <v>45197</v>
+      </c>
+      <c r="E21" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" t="s">
+        <v>108</v>
+      </c>
+      <c r="G21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="2">
+        <v>69.989999999999995</v>
+      </c>
+      <c r="I21">
+        <v>10114</v>
+      </c>
+      <c r="J21">
+        <v>79239</v>
+      </c>
+      <c r="K21" t="s">
+        <v>109</v>
+      </c>
+      <c r="L21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>26</v>
+      </c>
+      <c r="D22" s="1">
+        <v>45309</v>
+      </c>
+      <c r="E22" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" t="s">
+        <v>113</v>
+      </c>
+      <c r="G22" t="s">
+        <v>113</v>
+      </c>
+      <c r="H22" s="2">
+        <v>29.99</v>
+      </c>
+      <c r="I22">
+        <v>8231</v>
+      </c>
+      <c r="J22">
+        <v>269281</v>
+      </c>
+      <c r="K22" t="s">
+        <v>114</v>
+      </c>
+      <c r="L22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>44579</v>
+      </c>
+      <c r="E23" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23" t="s">
+        <v>119</v>
+      </c>
+      <c r="G23" t="s">
+        <v>119</v>
+      </c>
+      <c r="H23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23">
+        <v>1014</v>
+      </c>
+      <c r="J23">
+        <v>75171</v>
+      </c>
+      <c r="K23" t="s">
+        <v>120</v>
+      </c>
+      <c r="L23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24">
+        <v>13</v>
+      </c>
+      <c r="C24">
+        <v>453</v>
+      </c>
+      <c r="D24" s="1">
+        <v>42339</v>
+      </c>
+      <c r="E24" t="s">
+        <v>123</v>
+      </c>
+      <c r="F24" t="s">
+        <v>124</v>
+      </c>
+      <c r="G24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H24" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="I24">
+        <v>10402</v>
+      </c>
+      <c r="J24">
+        <v>1107988</v>
+      </c>
+      <c r="K24" t="s">
+        <v>126</v>
+      </c>
+      <c r="L24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25">
+        <v>-5</v>
+      </c>
+      <c r="C25">
+        <v>22</v>
+      </c>
+      <c r="D25" s="1">
+        <v>42426</v>
+      </c>
+      <c r="E25" t="s">
+        <v>129</v>
+      </c>
+      <c r="F25" t="s">
+        <v>130</v>
+      </c>
+      <c r="G25" t="s">
+        <v>130</v>
+      </c>
+      <c r="H25" s="2">
+        <v>14.99</v>
+      </c>
+      <c r="I25">
+        <v>16701</v>
+      </c>
+      <c r="J25">
+        <v>626295</v>
+      </c>
+      <c r="K25" t="s">
+        <v>131</v>
+      </c>
+      <c r="L25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>85</v>
+      </c>
+      <c r="D26" s="1">
+        <v>41358</v>
+      </c>
+      <c r="E26" t="s">
+        <v>134</v>
+      </c>
+      <c r="F26" t="s">
+        <v>135</v>
+      </c>
+      <c r="G26" t="s">
+        <v>135</v>
+      </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26">
+        <v>5035</v>
+      </c>
+      <c r="J26">
+        <v>584441</v>
+      </c>
+      <c r="K26" t="s">
+        <v>136</v>
+      </c>
+      <c r="L26" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>473</v>
+      </c>
+      <c r="D27" s="1">
+        <v>43139</v>
+      </c>
+      <c r="E27" t="s">
+        <v>139</v>
+      </c>
+      <c r="F27" t="s">
+        <v>140</v>
+      </c>
+      <c r="G27" t="s">
+        <v>140</v>
+      </c>
+      <c r="H27" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="I27">
+        <v>13837</v>
+      </c>
+      <c r="J27">
+        <v>897726</v>
+      </c>
+      <c r="K27" t="s">
+        <v>141</v>
+      </c>
+      <c r="L27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>45284</v>
+      </c>
+      <c r="E28" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" t="s">
+        <v>144</v>
+      </c>
+      <c r="G28" t="s">
+        <v>144</v>
+      </c>
+      <c r="H28" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28">
+        <v>930</v>
+      </c>
+      <c r="J28">
+        <v>4389</v>
+      </c>
+      <c r="K28" t="s">
+        <v>145</v>
+      </c>
+      <c r="L28" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>147</v>
+      </c>
+      <c r="B29">
+        <v>-5</v>
+      </c>
+      <c r="C29">
+        <v>381</v>
+      </c>
+      <c r="D29" s="1">
+        <v>42535</v>
+      </c>
+      <c r="E29" t="s">
+        <v>123</v>
+      </c>
+      <c r="F29" t="s">
+        <v>148</v>
+      </c>
+      <c r="G29" t="s">
+        <v>148</v>
+      </c>
+      <c r="H29" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="I29">
+        <v>5492</v>
+      </c>
+      <c r="J29">
+        <v>531801</v>
+      </c>
+      <c r="K29" t="s">
+        <v>149</v>
+      </c>
+      <c r="L29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>151</v>
+      </c>
+      <c r="B30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>45148</v>
+      </c>
+      <c r="E30" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" t="s">
+        <v>152</v>
+      </c>
+      <c r="G30" t="s">
+        <v>152</v>
+      </c>
+      <c r="H30" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30">
+        <v>9473</v>
+      </c>
+      <c r="J30">
+        <v>283116</v>
+      </c>
+      <c r="K30" t="s">
+        <v>153</v>
+      </c>
+      <c r="L30" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>155</v>
+      </c>
+      <c r="B31">
+        <v>-4</v>
+      </c>
+      <c r="C31">
+        <v>29</v>
+      </c>
+      <c r="D31" s="1">
+        <v>41688</v>
+      </c>
+      <c r="E31" t="s">
+        <v>156</v>
+      </c>
+      <c r="F31" t="s">
+        <v>157</v>
+      </c>
+      <c r="G31" t="s">
+        <v>157</v>
+      </c>
+      <c r="H31" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="I31">
+        <v>1182</v>
+      </c>
+      <c r="J31">
+        <v>69399</v>
+      </c>
+      <c r="K31" t="s">
+        <v>158</v>
+      </c>
+      <c r="L31" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>160</v>
+      </c>
+      <c r="B32">
+        <v>-13</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1">
+        <v>42142</v>
+      </c>
+      <c r="E32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" t="s">
+        <v>73</v>
+      </c>
+      <c r="H32" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="I32">
+        <v>8942</v>
+      </c>
+      <c r="J32">
+        <v>718431</v>
+      </c>
+      <c r="K32" t="s">
+        <v>161</v>
+      </c>
+      <c r="L32" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>163</v>
+      </c>
+      <c r="B33">
+        <v>-10</v>
+      </c>
+      <c r="C33">
+        <v>9</v>
+      </c>
+      <c r="D33" s="1">
+        <v>41200</v>
+      </c>
+      <c r="E33" t="s">
+        <v>164</v>
+      </c>
+      <c r="F33" t="s">
+        <v>165</v>
+      </c>
+      <c r="G33" t="s">
+        <v>165</v>
+      </c>
+      <c r="H33" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="I33">
+        <v>13778</v>
+      </c>
+      <c r="J33">
+        <v>584173</v>
+      </c>
+      <c r="K33" t="s">
+        <v>166</v>
+      </c>
+      <c r="L33" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>168</v>
+      </c>
+      <c r="B34">
+        <v>-12</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1">
+        <v>44967</v>
+      </c>
+      <c r="E34" t="s">
+        <v>87</v>
+      </c>
+      <c r="F34" t="s">
+        <v>169</v>
+      </c>
+      <c r="G34" t="s">
+        <v>170</v>
+      </c>
+      <c r="H34" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I34">
+        <v>4645</v>
+      </c>
+      <c r="J34">
+        <v>197179</v>
+      </c>
+      <c r="K34" t="s">
+        <v>171</v>
+      </c>
+      <c r="L34" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>173</v>
+      </c>
+      <c r="B35">
+        <v>-9</v>
+      </c>
+      <c r="C35">
+        <v>151</v>
+      </c>
+      <c r="D35" s="1">
+        <v>44508</v>
+      </c>
+      <c r="E35" t="s">
+        <v>174</v>
+      </c>
+      <c r="F35" t="s">
+        <v>102</v>
+      </c>
+      <c r="G35" t="s">
+        <v>103</v>
+      </c>
+      <c r="H35" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I35">
+        <v>5396</v>
+      </c>
+      <c r="J35">
+        <v>172206</v>
+      </c>
+      <c r="K35" t="s">
+        <v>175</v>
+      </c>
+      <c r="L35" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>177</v>
+      </c>
+      <c r="B36">
+        <v>-4</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36" s="1">
+        <v>45456</v>
+      </c>
+      <c r="E36" t="s">
+        <v>87</v>
+      </c>
+      <c r="F36" t="s">
+        <v>157</v>
+      </c>
+      <c r="G36" t="s">
+        <v>157</v>
+      </c>
+      <c r="H36" s="2">
+        <v>49.99</v>
+      </c>
+      <c r="I36">
+        <v>1272</v>
+      </c>
+      <c r="J36">
+        <v>3736</v>
+      </c>
+      <c r="K36" t="s">
+        <v>178</v>
+      </c>
+      <c r="L36" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1">
+        <v>45343</v>
+      </c>
+      <c r="E37" t="s">
+        <v>181</v>
+      </c>
+      <c r="F37" t="s">
+        <v>182</v>
+      </c>
+      <c r="G37" t="s">
+        <v>182</v>
+      </c>
+      <c r="H37" s="2">
+        <v>34.99</v>
+      </c>
+      <c r="I37">
+        <v>2689</v>
+      </c>
+      <c r="J37">
+        <v>87344</v>
+      </c>
+      <c r="K37" t="s">
+        <v>183</v>
+      </c>
+      <c r="L37" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>185</v>
+      </c>
+      <c r="B38">
+        <v>15</v>
+      </c>
+      <c r="C38">
+        <v>105</v>
+      </c>
+      <c r="D38" s="1">
+        <v>44862</v>
+      </c>
+      <c r="E38" t="s">
+        <v>123</v>
+      </c>
+      <c r="F38" t="s">
+        <v>186</v>
+      </c>
+      <c r="G38" t="s">
+        <v>187</v>
+      </c>
+      <c r="H38" s="2">
+        <v>69.989999999999995</v>
+      </c>
+      <c r="I38">
+        <v>4781</v>
+      </c>
+      <c r="J38">
+        <v>323487</v>
+      </c>
+      <c r="K38" t="s">
+        <v>188</v>
+      </c>
+      <c r="L38" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>190</v>
+      </c>
+      <c r="B39">
+        <v>-11</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39" s="1">
+        <v>43545</v>
+      </c>
+      <c r="E39" t="s">
+        <v>81</v>
+      </c>
+      <c r="F39" t="s">
+        <v>547</v>
+      </c>
+      <c r="G39" t="s">
+        <v>192</v>
+      </c>
+      <c r="H39" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I39">
+        <v>4941</v>
+      </c>
+      <c r="J39">
+        <v>212001</v>
+      </c>
+      <c r="K39" t="s">
+        <v>193</v>
+      </c>
+      <c r="L39" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>195</v>
+      </c>
+      <c r="B40">
+        <v>-2</v>
+      </c>
+      <c r="C40">
+        <v>6</v>
+      </c>
+      <c r="D40" s="1">
+        <v>42663</v>
+      </c>
+      <c r="E40" t="s">
+        <v>196</v>
+      </c>
+      <c r="F40" t="s">
+        <v>197</v>
+      </c>
+      <c r="G40" t="s">
+        <v>198</v>
+      </c>
+      <c r="H40" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I40">
+        <v>5361</v>
+      </c>
+      <c r="J40">
+        <v>232717</v>
+      </c>
+      <c r="K40" t="s">
+        <v>199</v>
+      </c>
+      <c r="L40" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>201</v>
+      </c>
+      <c r="B41">
+        <v>-1</v>
+      </c>
+      <c r="C41">
+        <v>17</v>
+      </c>
+      <c r="D41" s="1">
+        <v>43935</v>
+      </c>
+      <c r="E41" t="s">
+        <v>72</v>
+      </c>
+      <c r="F41" t="s">
+        <v>202</v>
+      </c>
+      <c r="G41" t="s">
+        <v>203</v>
+      </c>
+      <c r="H41" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="I41">
+        <v>1410</v>
+      </c>
+      <c r="J41">
+        <v>60156</v>
+      </c>
+      <c r="K41" t="s">
+        <v>204</v>
+      </c>
+      <c r="L41" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>206</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42" s="1">
+        <v>45420</v>
+      </c>
+      <c r="E42" t="s">
+        <v>66</v>
+      </c>
+      <c r="F42" t="s">
+        <v>207</v>
+      </c>
+      <c r="G42" t="s">
+        <v>207</v>
+      </c>
+      <c r="H42" s="2">
+        <v>34.99</v>
+      </c>
+      <c r="I42">
+        <v>1995</v>
+      </c>
+      <c r="J42">
+        <v>84063</v>
+      </c>
+      <c r="K42" t="s">
+        <v>208</v>
+      </c>
+      <c r="L42" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>210</v>
+      </c>
+      <c r="B43">
+        <v>-13</v>
+      </c>
+      <c r="C43">
+        <v>195</v>
+      </c>
+      <c r="D43" s="1">
+        <v>41884</v>
+      </c>
+      <c r="E43" t="s">
+        <v>211</v>
+      </c>
+      <c r="F43" t="s">
+        <v>212</v>
+      </c>
+      <c r="G43" t="s">
+        <v>44</v>
+      </c>
+      <c r="H43" t="s">
+        <v>27</v>
+      </c>
+      <c r="I43">
+        <v>4215</v>
+      </c>
+      <c r="J43">
+        <v>144202</v>
+      </c>
+      <c r="K43" t="s">
+        <v>213</v>
+      </c>
+      <c r="L43" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>215</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <v>26</v>
+      </c>
+      <c r="D44" s="1">
+        <v>45330</v>
+      </c>
+      <c r="E44" t="s">
+        <v>123</v>
+      </c>
+      <c r="F44" t="s">
+        <v>216</v>
+      </c>
+      <c r="G44" t="s">
+        <v>217</v>
+      </c>
+      <c r="H44" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="I44">
+        <v>6261</v>
+      </c>
+      <c r="J44">
+        <v>652529</v>
+      </c>
+      <c r="K44" t="s">
+        <v>218</v>
+      </c>
+      <c r="L44" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>220</v>
+      </c>
+      <c r="B45">
+        <v>30</v>
+      </c>
+      <c r="C45">
+        <v>132</v>
+      </c>
+      <c r="D45" s="1">
+        <v>44603</v>
+      </c>
+      <c r="E45" t="s">
+        <v>221</v>
+      </c>
+      <c r="F45" t="s">
+        <v>222</v>
+      </c>
+      <c r="G45" t="s">
+        <v>223</v>
+      </c>
+      <c r="H45" t="s">
+        <v>27</v>
+      </c>
+      <c r="I45">
+        <v>571</v>
+      </c>
+      <c r="J45">
+        <v>200119</v>
+      </c>
+      <c r="K45" t="s">
+        <v>224</v>
+      </c>
+      <c r="L45" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>226</v>
+      </c>
+      <c r="B46">
+        <v>-10</v>
+      </c>
+      <c r="C46">
+        <v>73</v>
+      </c>
+      <c r="D46" s="1">
+        <v>45344</v>
+      </c>
+      <c r="E46" t="s">
+        <v>227</v>
+      </c>
+      <c r="F46" t="s">
+        <v>228</v>
+      </c>
+      <c r="G46" t="s">
+        <v>229</v>
+      </c>
+      <c r="H46" s="2">
+        <v>29.99</v>
+      </c>
+      <c r="I46">
+        <v>3732</v>
+      </c>
+      <c r="J46">
+        <v>178770</v>
+      </c>
+      <c r="K46" t="s">
+        <v>230</v>
+      </c>
+      <c r="L46" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>232</v>
+      </c>
+      <c r="B47">
+        <v>-12</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47" s="1">
+        <v>45194</v>
+      </c>
+      <c r="E47" t="s">
+        <v>72</v>
+      </c>
+      <c r="F47" t="s">
+        <v>73</v>
+      </c>
+      <c r="G47" t="s">
+        <v>73</v>
+      </c>
+      <c r="H47" s="2">
+        <v>29.99</v>
+      </c>
+      <c r="I47">
+        <v>462</v>
+      </c>
+      <c r="J47">
+        <v>15100</v>
+      </c>
+      <c r="L47" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>234</v>
+      </c>
+      <c r="B48" t="s">
+        <v>117</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1">
+        <v>42811</v>
+      </c>
+      <c r="E48" t="s">
+        <v>37</v>
+      </c>
+      <c r="F48" t="s">
+        <v>235</v>
+      </c>
+      <c r="G48" t="s">
+        <v>157</v>
+      </c>
+      <c r="H48" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="I48">
+        <v>1392</v>
+      </c>
+      <c r="J48">
+        <v>95841</v>
+      </c>
+      <c r="K48" t="s">
+        <v>236</v>
+      </c>
+      <c r="L48" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>238</v>
+      </c>
+      <c r="B49">
+        <v>7</v>
+      </c>
+      <c r="C49">
+        <v>495</v>
+      </c>
+      <c r="D49" s="1">
+        <v>41733</v>
+      </c>
+      <c r="E49" t="s">
+        <v>239</v>
+      </c>
+      <c r="F49" t="s">
+        <v>240</v>
+      </c>
+      <c r="G49" t="s">
+        <v>203</v>
+      </c>
+      <c r="H49" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="I49">
+        <v>764</v>
+      </c>
+      <c r="J49">
+        <v>121812</v>
+      </c>
+      <c r="K49" t="s">
+        <v>241</v>
+      </c>
+      <c r="L49" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>243</v>
+      </c>
+      <c r="B50">
+        <v>34</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50" s="1">
+        <v>45187</v>
+      </c>
+      <c r="E50" t="s">
+        <v>87</v>
+      </c>
+      <c r="F50" t="s">
+        <v>244</v>
+      </c>
+      <c r="G50" t="s">
+        <v>244</v>
+      </c>
+      <c r="H50" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I50">
+        <v>1733</v>
+      </c>
+      <c r="J50">
+        <v>28916</v>
+      </c>
+      <c r="K50" t="s">
+        <v>245</v>
+      </c>
+      <c r="L50" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>247</v>
+      </c>
+      <c r="B51">
+        <v>16</v>
+      </c>
+      <c r="C51">
+        <v>6</v>
+      </c>
+      <c r="D51" s="1">
+        <v>45450</v>
+      </c>
+      <c r="E51" t="s">
+        <v>248</v>
+      </c>
+      <c r="F51" t="s">
+        <v>249</v>
+      </c>
+      <c r="G51" t="s">
+        <v>249</v>
+      </c>
+      <c r="H51" t="s">
+        <v>15</v>
+      </c>
+      <c r="I51">
+        <v>11607</v>
+      </c>
+      <c r="J51">
+        <v>38298</v>
+      </c>
+      <c r="K51" t="s">
+        <v>250</v>
+      </c>
+      <c r="L51" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>252</v>
+      </c>
+      <c r="B52">
+        <v>-18</v>
+      </c>
+      <c r="C52">
+        <v>12</v>
+      </c>
+      <c r="D52" s="1">
+        <v>45408</v>
+      </c>
+      <c r="E52" t="s">
+        <v>253</v>
+      </c>
+      <c r="F52" t="s">
+        <v>254</v>
+      </c>
+      <c r="G52" t="s">
+        <v>255</v>
+      </c>
+      <c r="H52" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="I52">
+        <v>2492</v>
+      </c>
+      <c r="J52">
+        <v>44649</v>
+      </c>
+      <c r="K52" t="s">
+        <v>256</v>
+      </c>
+      <c r="L52" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>258</v>
+      </c>
+      <c r="B53">
+        <v>-1</v>
+      </c>
+      <c r="C53">
+        <v>177</v>
+      </c>
+      <c r="D53" s="1">
+        <v>42879</v>
+      </c>
+      <c r="E53" t="s">
+        <v>259</v>
+      </c>
+      <c r="F53" t="s">
+        <v>260</v>
+      </c>
+      <c r="G53" t="s">
+        <v>260</v>
+      </c>
+      <c r="H53" s="2">
+        <v>9.99</v>
+      </c>
+      <c r="I53">
+        <v>744</v>
+      </c>
+      <c r="J53">
+        <v>55695</v>
+      </c>
+      <c r="K53" t="s">
+        <v>261</v>
+      </c>
+      <c r="L53" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>263</v>
+      </c>
+      <c r="B54">
+        <v>-7</v>
+      </c>
+      <c r="C54">
+        <v>10</v>
+      </c>
+      <c r="D54" s="1">
+        <v>45078</v>
+      </c>
+      <c r="E54" t="s">
+        <v>81</v>
+      </c>
+      <c r="F54" t="s">
+        <v>264</v>
+      </c>
+      <c r="G54" t="s">
+        <v>264</v>
+      </c>
+      <c r="H54" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I54">
+        <v>1560</v>
+      </c>
+      <c r="J54">
+        <v>27593</v>
+      </c>
+      <c r="K54" t="s">
+        <v>265</v>
+      </c>
+      <c r="L54" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>267</v>
+      </c>
+      <c r="B55">
+        <v>-5</v>
+      </c>
+      <c r="C55">
+        <v>22</v>
+      </c>
+      <c r="D55" s="1">
+        <v>43985</v>
+      </c>
+      <c r="E55" t="s">
+        <v>81</v>
+      </c>
+      <c r="F55" t="s">
+        <v>268</v>
+      </c>
+      <c r="G55" t="s">
+        <v>103</v>
+      </c>
+      <c r="H55" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="I55">
+        <v>3695</v>
+      </c>
+      <c r="J55">
+        <v>289121</v>
+      </c>
+      <c r="K55" t="s">
+        <v>269</v>
+      </c>
+      <c r="L55" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>271</v>
+      </c>
+      <c r="B56">
+        <v>-12</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+      <c r="D56" s="1">
+        <v>42402</v>
+      </c>
+      <c r="E56" t="s">
+        <v>164</v>
+      </c>
+      <c r="F56" t="s">
+        <v>165</v>
+      </c>
+      <c r="G56" t="s">
+        <v>165</v>
+      </c>
+      <c r="H56" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="I56">
+        <v>3136</v>
+      </c>
+      <c r="J56">
+        <v>127905</v>
+      </c>
+      <c r="K56" t="s">
+        <v>272</v>
+      </c>
+      <c r="L56" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>274</v>
+      </c>
+      <c r="B57">
+        <v>-18</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57" s="1">
+        <v>44608</v>
+      </c>
+      <c r="E57" t="s">
+        <v>275</v>
+      </c>
+      <c r="F57" t="s">
+        <v>276</v>
+      </c>
+      <c r="G57" t="s">
+        <v>277</v>
+      </c>
+      <c r="H57" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I57">
+        <v>1663</v>
+      </c>
+      <c r="J57">
+        <v>73803</v>
+      </c>
+      <c r="K57" t="s">
+        <v>278</v>
+      </c>
+      <c r="L57" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>280</v>
+      </c>
+      <c r="B58">
+        <v>-15</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58" s="1">
+        <v>44519</v>
+      </c>
+      <c r="E58" t="s">
+        <v>281</v>
+      </c>
+      <c r="F58" t="s">
+        <v>282</v>
+      </c>
+      <c r="G58" t="s">
+        <v>44</v>
+      </c>
+      <c r="H58" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I58">
+        <v>5330</v>
+      </c>
+      <c r="J58">
+        <v>208997</v>
+      </c>
+      <c r="K58" t="s">
+        <v>548</v>
+      </c>
+      <c r="L58" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>285</v>
+      </c>
+      <c r="B59">
+        <v>-13</v>
+      </c>
+      <c r="C59">
+        <v>19</v>
+      </c>
+      <c r="D59" s="1">
+        <v>45240</v>
+      </c>
+      <c r="E59" t="s">
+        <v>123</v>
+      </c>
+      <c r="F59" t="s">
+        <v>186</v>
+      </c>
+      <c r="G59" t="s">
+        <v>187</v>
+      </c>
+      <c r="H59" s="2">
+        <v>69.989999999999995</v>
+      </c>
+      <c r="I59">
+        <v>497</v>
+      </c>
+      <c r="J59">
+        <v>10083</v>
+      </c>
+      <c r="K59" t="s">
+        <v>286</v>
+      </c>
+      <c r="L59" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>288</v>
+      </c>
+      <c r="B60">
+        <v>-19</v>
+      </c>
+      <c r="C60">
+        <v>3</v>
+      </c>
+      <c r="D60" s="1">
+        <v>45273</v>
+      </c>
+      <c r="E60" t="s">
+        <v>289</v>
+      </c>
+      <c r="F60" t="s">
+        <v>290</v>
+      </c>
+      <c r="G60" t="s">
+        <v>290</v>
+      </c>
+      <c r="H60" s="2">
+        <v>49.99</v>
+      </c>
+      <c r="I60">
+        <v>4329</v>
+      </c>
+      <c r="J60">
+        <v>145278</v>
+      </c>
+      <c r="K60" t="s">
+        <v>291</v>
+      </c>
+      <c r="L60" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>293</v>
+      </c>
+      <c r="B61">
+        <v>7</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61" s="1">
+        <v>44092</v>
+      </c>
+      <c r="E61" t="s">
+        <v>294</v>
+      </c>
+      <c r="F61" t="s">
+        <v>295</v>
+      </c>
+      <c r="G61" t="s">
+        <v>295</v>
+      </c>
+      <c r="H61" s="2">
+        <v>13.99</v>
+      </c>
+      <c r="I61">
+        <v>9835</v>
+      </c>
+      <c r="J61">
+        <v>564258</v>
+      </c>
+      <c r="K61" t="s">
+        <v>296</v>
+      </c>
+      <c r="L61" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>298</v>
+      </c>
+      <c r="B62">
+        <v>12</v>
+      </c>
+      <c r="C62">
+        <v>12</v>
+      </c>
+      <c r="D62" s="1">
+        <v>45428</v>
+      </c>
+      <c r="E62" t="s">
+        <v>81</v>
+      </c>
+      <c r="F62" t="s">
+        <v>299</v>
+      </c>
+      <c r="G62" t="s">
+        <v>217</v>
+      </c>
+      <c r="H62" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I62">
+        <v>2786</v>
+      </c>
+      <c r="J62">
+        <v>23946</v>
+      </c>
+      <c r="K62" t="s">
+        <v>300</v>
+      </c>
+      <c r="L62" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>302</v>
+      </c>
+      <c r="B63" t="s">
+        <v>48</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" s="1">
+        <v>45539</v>
+      </c>
+      <c r="E63" t="s">
+        <v>196</v>
+      </c>
+      <c r="F63" t="s">
+        <v>303</v>
+      </c>
+      <c r="G63" t="s">
+        <v>103</v>
+      </c>
+      <c r="H63" s="2">
+        <v>24.99</v>
+      </c>
+      <c r="K63" t="s">
+        <v>304</v>
+      </c>
+      <c r="L63" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>306</v>
+      </c>
+      <c r="B64" t="s">
+        <v>117</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64" s="1">
+        <v>43846</v>
+      </c>
+      <c r="E64" t="s">
+        <v>37</v>
+      </c>
+      <c r="F64" t="s">
+        <v>307</v>
+      </c>
+      <c r="G64" t="s">
+        <v>308</v>
+      </c>
+      <c r="H64" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I64">
+        <v>753</v>
+      </c>
+      <c r="J64">
+        <v>38190</v>
+      </c>
+      <c r="K64" t="s">
+        <v>309</v>
+      </c>
+      <c r="L64" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>311</v>
+      </c>
+      <c r="B65" t="s">
+        <v>117</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65" s="1">
+        <v>39365</v>
+      </c>
+      <c r="E65" t="s">
+        <v>31</v>
+      </c>
+      <c r="F65" t="s">
+        <v>20</v>
+      </c>
+      <c r="G65" t="s">
+        <v>20</v>
+      </c>
+      <c r="H65" t="s">
+        <v>15</v>
+      </c>
+      <c r="I65">
+        <v>10794</v>
+      </c>
+      <c r="J65">
+        <v>1110984</v>
+      </c>
+      <c r="K65" t="s">
+        <v>312</v>
+      </c>
+      <c r="L65" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>314</v>
+      </c>
+      <c r="B66" t="s">
+        <v>48</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66" s="1">
+        <v>45484</v>
+      </c>
+      <c r="E66" t="s">
+        <v>315</v>
+      </c>
+      <c r="F66" t="s">
+        <v>316</v>
+      </c>
+      <c r="G66" t="s">
+        <v>317</v>
+      </c>
+      <c r="H66" s="2">
+        <v>24.99</v>
+      </c>
+      <c r="I66">
+        <v>1066</v>
+      </c>
+      <c r="K66" t="s">
+        <v>318</v>
+      </c>
+      <c r="L66" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>320</v>
+      </c>
+      <c r="B67">
+        <v>-8</v>
+      </c>
+      <c r="C67">
+        <v>3</v>
+      </c>
+      <c r="D67" s="1">
+        <v>43390</v>
+      </c>
+      <c r="E67" t="s">
+        <v>321</v>
+      </c>
+      <c r="F67" t="s">
+        <v>322</v>
+      </c>
+      <c r="G67" t="s">
+        <v>322</v>
+      </c>
+      <c r="H67" s="2">
+        <v>49.99</v>
+      </c>
+      <c r="I67">
+        <v>2017</v>
+      </c>
+      <c r="J67">
+        <v>161126</v>
+      </c>
+      <c r="K67" t="s">
+        <v>323</v>
+      </c>
+      <c r="L67" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>325</v>
+      </c>
+      <c r="B68">
+        <v>-13</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
+      </c>
+      <c r="D68" s="1">
+        <v>45342</v>
+      </c>
+      <c r="E68" t="s">
+        <v>326</v>
+      </c>
+      <c r="F68" t="s">
+        <v>327</v>
+      </c>
+      <c r="G68" t="s">
+        <v>327</v>
+      </c>
+      <c r="H68" s="2">
+        <v>12.99</v>
+      </c>
+      <c r="I68">
+        <v>5774</v>
+      </c>
+      <c r="J68">
+        <v>42434</v>
+      </c>
+      <c r="K68" t="s">
+        <v>328</v>
+      </c>
+      <c r="L68" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>330</v>
+      </c>
+      <c r="B69">
+        <v>-15</v>
+      </c>
+      <c r="C69">
+        <v>3</v>
+      </c>
+      <c r="D69" s="1">
+        <v>45105</v>
+      </c>
+      <c r="E69" t="s">
+        <v>331</v>
+      </c>
+      <c r="F69" t="s">
+        <v>332</v>
+      </c>
+      <c r="G69" t="s">
+        <v>332</v>
+      </c>
+      <c r="H69" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="I69">
+        <v>4328</v>
+      </c>
+      <c r="J69">
+        <v>99391</v>
+      </c>
+      <c r="K69" t="s">
+        <v>333</v>
+      </c>
+      <c r="L69" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>335</v>
+      </c>
+      <c r="B70" t="s">
+        <v>117</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70" s="1">
+        <v>44595</v>
+      </c>
+      <c r="E70" t="s">
+        <v>87</v>
+      </c>
+      <c r="F70" t="s">
+        <v>336</v>
+      </c>
+      <c r="G70" t="s">
+        <v>336</v>
+      </c>
+      <c r="H70" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I70">
+        <v>2021</v>
+      </c>
+      <c r="J70">
+        <v>129291</v>
+      </c>
+      <c r="K70" t="s">
+        <v>337</v>
+      </c>
+      <c r="L70" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>339</v>
+      </c>
+      <c r="B71">
+        <v>19</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
+      </c>
+      <c r="D71" s="1">
+        <v>45222</v>
+      </c>
+      <c r="E71" t="s">
+        <v>340</v>
+      </c>
+      <c r="F71" t="s">
+        <v>341</v>
+      </c>
+      <c r="G71" t="s">
+        <v>341</v>
+      </c>
+      <c r="H71" s="2">
+        <v>9.99</v>
+      </c>
+      <c r="I71">
+        <v>9752</v>
+      </c>
+      <c r="J71">
+        <v>335990</v>
+      </c>
+      <c r="K71" t="s">
+        <v>342</v>
+      </c>
+      <c r="L71" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>344</v>
+      </c>
+      <c r="B72">
+        <v>-9</v>
+      </c>
+      <c r="C72">
+        <v>3</v>
+      </c>
+      <c r="D72" s="1">
+        <v>42527</v>
+      </c>
+      <c r="E72" t="s">
+        <v>345</v>
+      </c>
+      <c r="F72" t="s">
+        <v>346</v>
+      </c>
+      <c r="G72" t="s">
+        <v>347</v>
+      </c>
+      <c r="H72" s="2">
+        <v>49.99</v>
+      </c>
+      <c r="I72">
+        <v>3581</v>
+      </c>
+      <c r="J72">
+        <v>213479</v>
+      </c>
+      <c r="K72" t="s">
+        <v>348</v>
+      </c>
+      <c r="L72" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>350</v>
+      </c>
+      <c r="B73">
+        <v>-1</v>
+      </c>
+      <c r="C73">
+        <v>3</v>
+      </c>
+      <c r="D73" s="1">
+        <v>45324</v>
+      </c>
+      <c r="E73" t="s">
+        <v>54</v>
+      </c>
+      <c r="F73" t="s">
+        <v>351</v>
+      </c>
+      <c r="G73" t="s">
+        <v>277</v>
+      </c>
+      <c r="H73" s="2">
+        <v>69.989999999999995</v>
+      </c>
+      <c r="I73">
+        <v>1067</v>
+      </c>
+      <c r="J73">
+        <v>17048</v>
+      </c>
+      <c r="K73" t="s">
+        <v>352</v>
+      </c>
+      <c r="L73" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>354</v>
+      </c>
+      <c r="B74">
+        <v>-32</v>
+      </c>
+      <c r="C74">
+        <v>3</v>
+      </c>
+      <c r="D74" s="1">
+        <v>44949</v>
+      </c>
+      <c r="E74" t="s">
+        <v>81</v>
+      </c>
+      <c r="F74" t="s">
+        <v>355</v>
+      </c>
+      <c r="G74" t="s">
+        <v>125</v>
+      </c>
+      <c r="H74" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I74">
+        <v>2997</v>
+      </c>
+      <c r="J74">
+        <v>20547</v>
+      </c>
+      <c r="K74" t="s">
+        <v>356</v>
+      </c>
+      <c r="L74" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>358</v>
+      </c>
+      <c r="B75">
+        <v>-15</v>
+      </c>
+      <c r="C75">
+        <v>14</v>
+      </c>
+      <c r="D75" s="1">
+        <v>42499</v>
+      </c>
+      <c r="E75" t="s">
+        <v>345</v>
+      </c>
+      <c r="F75" t="s">
+        <v>346</v>
+      </c>
+      <c r="G75" t="s">
+        <v>347</v>
+      </c>
+      <c r="H75" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="I75">
+        <v>1054</v>
+      </c>
+      <c r="J75">
+        <v>117985</v>
+      </c>
+      <c r="K75" t="s">
+        <v>359</v>
+      </c>
+      <c r="L75" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>361</v>
+      </c>
+      <c r="B76">
+        <v>-31</v>
+      </c>
+      <c r="C76">
+        <v>3</v>
+      </c>
+      <c r="D76" s="1">
+        <v>44509</v>
+      </c>
+      <c r="E76" t="s">
+        <v>345</v>
+      </c>
+      <c r="F76" t="s">
+        <v>362</v>
+      </c>
+      <c r="G76" t="s">
+        <v>362</v>
+      </c>
+      <c r="H76" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I76">
+        <v>1773</v>
+      </c>
+      <c r="J76">
+        <v>24635</v>
+      </c>
+      <c r="K76" t="s">
+        <v>363</v>
+      </c>
+      <c r="L76" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>365</v>
+      </c>
+      <c r="B77">
+        <v>-28</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77" s="1">
+        <v>42314</v>
+      </c>
+      <c r="E77" t="s">
+        <v>81</v>
+      </c>
+      <c r="F77" t="s">
+        <v>366</v>
+      </c>
+      <c r="G77" t="s">
+        <v>187</v>
+      </c>
+      <c r="H77" s="2">
+        <v>14.99</v>
+      </c>
+      <c r="I77">
+        <v>2516</v>
+      </c>
+      <c r="J77">
+        <v>128812</v>
+      </c>
+      <c r="K77" t="s">
+        <v>367</v>
+      </c>
+      <c r="L77" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>369</v>
+      </c>
+      <c r="B78" t="s">
+        <v>117</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78" s="3">
+        <v>43405</v>
+      </c>
+      <c r="E78" t="s">
+        <v>370</v>
+      </c>
+      <c r="F78" t="s">
+        <v>371</v>
+      </c>
+      <c r="G78" t="s">
+        <v>371</v>
+      </c>
+      <c r="H78" s="2">
+        <v>3.99</v>
+      </c>
+      <c r="I78">
+        <v>11948</v>
+      </c>
+      <c r="J78">
+        <v>741388</v>
+      </c>
+      <c r="K78" t="s">
+        <v>372</v>
+      </c>
+      <c r="L78" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>374</v>
+      </c>
+      <c r="B79">
+        <v>-14</v>
+      </c>
+      <c r="C79">
+        <v>3</v>
+      </c>
+      <c r="D79" s="1">
+        <v>41586</v>
+      </c>
+      <c r="E79" t="s">
+        <v>375</v>
+      </c>
+      <c r="F79" t="s">
+        <v>376</v>
+      </c>
+      <c r="G79" t="s">
+        <v>376</v>
+      </c>
+      <c r="H79" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="I79">
+        <v>6027</v>
+      </c>
+      <c r="J79">
+        <v>235042</v>
+      </c>
+      <c r="K79" t="s">
+        <v>377</v>
+      </c>
+      <c r="L79" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>379</v>
+      </c>
+      <c r="B80">
+        <v>-11</v>
+      </c>
+      <c r="C80">
+        <v>3</v>
+      </c>
+      <c r="D80" s="1">
+        <v>43320</v>
+      </c>
+      <c r="E80" t="s">
+        <v>123</v>
+      </c>
+      <c r="F80" t="s">
+        <v>264</v>
+      </c>
+      <c r="G80" t="s">
+        <v>264</v>
+      </c>
+      <c r="H80" s="2">
+        <v>29.99</v>
+      </c>
+      <c r="I80">
+        <v>3256</v>
+      </c>
+      <c r="J80">
+        <v>270499</v>
+      </c>
+      <c r="K80" t="s">
+        <v>380</v>
+      </c>
+      <c r="L80" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>382</v>
+      </c>
+      <c r="B81">
+        <v>-15</v>
+      </c>
+      <c r="C81">
+        <v>3</v>
+      </c>
+      <c r="D81" s="1">
+        <v>44280</v>
+      </c>
+      <c r="E81" t="s">
+        <v>81</v>
+      </c>
+      <c r="F81" t="s">
+        <v>383</v>
+      </c>
+      <c r="G81" t="s">
+        <v>44</v>
+      </c>
+      <c r="H81" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="I81">
+        <v>3010</v>
+      </c>
+      <c r="J81">
+        <v>145927</v>
+      </c>
+      <c r="K81" t="s">
+        <v>384</v>
+      </c>
+      <c r="L81" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>386</v>
+      </c>
+      <c r="B82">
+        <v>-20</v>
+      </c>
+      <c r="C82">
+        <v>4</v>
+      </c>
+      <c r="D82" s="1">
+        <v>44581</v>
+      </c>
+      <c r="E82" t="s">
+        <v>81</v>
+      </c>
+      <c r="F82" t="s">
+        <v>387</v>
+      </c>
+      <c r="G82" t="s">
+        <v>387</v>
+      </c>
+      <c r="H82" s="2">
+        <v>29.99</v>
+      </c>
+      <c r="I82">
+        <v>2232</v>
+      </c>
+      <c r="J82">
+        <v>24901</v>
+      </c>
+      <c r="K82" t="s">
+        <v>388</v>
+      </c>
+      <c r="L82" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>390</v>
+      </c>
+      <c r="B83">
+        <v>18</v>
+      </c>
+      <c r="C83">
+        <v>6</v>
+      </c>
+      <c r="D83" s="1">
+        <v>45450</v>
+      </c>
+      <c r="E83" t="s">
+        <v>391</v>
+      </c>
+      <c r="F83" t="s">
+        <v>392</v>
+      </c>
+      <c r="G83" t="s">
+        <v>392</v>
+      </c>
+      <c r="H83" s="2">
+        <v>33.32</v>
+      </c>
+      <c r="I83">
+        <v>3609</v>
+      </c>
+      <c r="J83">
+        <v>19133</v>
+      </c>
+      <c r="K83" t="s">
+        <v>393</v>
+      </c>
+      <c r="L83" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>395</v>
+      </c>
+      <c r="B84">
+        <v>-13</v>
+      </c>
+      <c r="C84">
+        <v>3</v>
+      </c>
+      <c r="D84" s="1">
+        <v>45162</v>
+      </c>
+      <c r="E84" t="s">
+        <v>123</v>
+      </c>
+      <c r="F84" t="s">
+        <v>547</v>
+      </c>
+      <c r="G84" t="s">
+        <v>547</v>
+      </c>
+      <c r="H84" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I84">
+        <v>1197</v>
+      </c>
+      <c r="J84">
+        <v>54315</v>
+      </c>
+      <c r="K84" t="s">
+        <v>396</v>
+      </c>
+      <c r="L84" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>398</v>
+      </c>
+      <c r="B85">
+        <v>-6</v>
+      </c>
+      <c r="C85">
+        <v>3</v>
+      </c>
+      <c r="D85" s="1">
+        <v>44075</v>
+      </c>
+      <c r="E85" t="s">
+        <v>399</v>
+      </c>
+      <c r="F85" t="s">
+        <v>346</v>
+      </c>
+      <c r="G85" t="s">
+        <v>347</v>
+      </c>
+      <c r="H85" s="2">
+        <v>49.99</v>
+      </c>
+      <c r="I85">
+        <v>942</v>
+      </c>
+      <c r="J85">
+        <v>71316</v>
+      </c>
+      <c r="K85" t="s">
+        <v>400</v>
+      </c>
+      <c r="L85" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>402</v>
+      </c>
+      <c r="B86">
+        <v>-5</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86" s="1">
+        <v>44060</v>
+      </c>
+      <c r="E86" t="s">
+        <v>403</v>
+      </c>
+      <c r="F86" t="s">
+        <v>404</v>
+      </c>
+      <c r="G86" t="s">
+        <v>103</v>
+      </c>
+      <c r="H86" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I86">
+        <v>1081</v>
+      </c>
+      <c r="J86">
+        <v>57341</v>
+      </c>
+      <c r="K86" t="s">
+        <v>405</v>
+      </c>
+      <c r="L86" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>407</v>
+      </c>
+      <c r="B87">
+        <v>-5</v>
+      </c>
+      <c r="C87">
+        <v>2</v>
+      </c>
+      <c r="D87" s="1">
+        <v>44732</v>
+      </c>
+      <c r="E87" t="s">
+        <v>408</v>
+      </c>
+      <c r="F87" t="s">
+        <v>409</v>
+      </c>
+      <c r="G87" t="s">
+        <v>410</v>
+      </c>
+      <c r="H87" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="I87">
+        <v>3950</v>
+      </c>
+      <c r="J87">
+        <v>271798</v>
+      </c>
+      <c r="K87" t="s">
+        <v>411</v>
+      </c>
+      <c r="L87" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>413</v>
+      </c>
+      <c r="B88">
+        <v>-24</v>
+      </c>
+      <c r="C88">
+        <v>3</v>
+      </c>
+      <c r="D88" s="1">
+        <v>45322</v>
+      </c>
+      <c r="E88" t="s">
+        <v>87</v>
+      </c>
+      <c r="F88" t="s">
+        <v>414</v>
+      </c>
+      <c r="G88" t="s">
+        <v>414</v>
+      </c>
+      <c r="H88" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I88">
+        <v>748</v>
+      </c>
+      <c r="J88">
+        <v>30962</v>
+      </c>
+      <c r="K88" t="s">
+        <v>415</v>
+      </c>
+      <c r="L88" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>417</v>
+      </c>
+      <c r="B89">
+        <v>-32</v>
+      </c>
+      <c r="C89">
+        <v>4</v>
+      </c>
+      <c r="D89" s="1">
+        <v>45372</v>
+      </c>
+      <c r="E89" t="s">
+        <v>37</v>
+      </c>
+      <c r="F89" t="s">
+        <v>418</v>
+      </c>
+      <c r="G89" t="s">
+        <v>217</v>
+      </c>
+      <c r="H89" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I89">
+        <v>1010</v>
+      </c>
+      <c r="J89">
+        <v>9960</v>
+      </c>
+      <c r="K89" t="s">
+        <v>419</v>
+      </c>
+      <c r="L89" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>421</v>
+      </c>
+      <c r="B90">
+        <v>-39</v>
+      </c>
+      <c r="C90">
+        <v>3</v>
+      </c>
+      <c r="D90" s="1">
+        <v>43413</v>
+      </c>
+      <c r="E90" t="s">
+        <v>123</v>
+      </c>
+      <c r="F90" t="s">
+        <v>282</v>
+      </c>
+      <c r="G90" t="s">
+        <v>44</v>
+      </c>
+      <c r="H90" s="2">
+        <v>49.99</v>
+      </c>
+      <c r="I90">
+        <v>7579</v>
+      </c>
+      <c r="J90">
+        <v>189667</v>
+      </c>
+      <c r="K90" t="s">
+        <v>422</v>
+      </c>
+      <c r="L90" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>424</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>2</v>
+      </c>
+      <c r="D91" s="1">
+        <v>45383</v>
+      </c>
+      <c r="E91" t="s">
+        <v>289</v>
+      </c>
+      <c r="F91" t="s">
+        <v>425</v>
+      </c>
+      <c r="G91" t="s">
+        <v>549</v>
+      </c>
+      <c r="H91" s="2">
+        <v>7.99</v>
+      </c>
+      <c r="I91">
+        <v>4998</v>
+      </c>
+      <c r="J91">
+        <v>29049</v>
+      </c>
+      <c r="K91" t="s">
+        <v>427</v>
+      </c>
+      <c r="L91" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>429</v>
+      </c>
+      <c r="B92" t="s">
+        <v>117</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92" s="1">
+        <v>43990</v>
+      </c>
+      <c r="E92" t="s">
+        <v>430</v>
+      </c>
+      <c r="F92" t="s">
+        <v>431</v>
+      </c>
+      <c r="G92" t="s">
+        <v>432</v>
+      </c>
+      <c r="H92" s="2">
+        <v>29.99</v>
+      </c>
+      <c r="I92">
+        <v>2757</v>
+      </c>
+      <c r="J92">
+        <v>141467</v>
+      </c>
+      <c r="K92" t="s">
+        <v>433</v>
+      </c>
+      <c r="L92" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>435</v>
+      </c>
+      <c r="B93">
+        <v>-16</v>
+      </c>
+      <c r="C93">
+        <v>3</v>
+      </c>
+      <c r="D93" s="1">
+        <v>45315</v>
+      </c>
+      <c r="E93" t="s">
+        <v>436</v>
+      </c>
+      <c r="F93" t="s">
+        <v>437</v>
+      </c>
+      <c r="G93" t="s">
+        <v>437</v>
+      </c>
+      <c r="H93" s="2">
+        <v>29.99</v>
+      </c>
+      <c r="I93">
+        <v>1356</v>
+      </c>
+      <c r="J93">
+        <v>47724</v>
+      </c>
+      <c r="K93" t="s">
+        <v>438</v>
+      </c>
+      <c r="L93" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>440</v>
+      </c>
+      <c r="B94">
+        <v>-24</v>
+      </c>
+      <c r="C94">
+        <v>3</v>
+      </c>
+      <c r="D94" s="1">
+        <v>42178</v>
+      </c>
+      <c r="E94" t="s">
+        <v>81</v>
+      </c>
+      <c r="F94" t="s">
+        <v>441</v>
+      </c>
+      <c r="G94" t="s">
+        <v>442</v>
+      </c>
+      <c r="H94" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="I94">
+        <v>3050</v>
+      </c>
+      <c r="J94">
+        <v>83953</v>
+      </c>
+      <c r="K94" t="s">
+        <v>443</v>
+      </c>
+      <c r="L94" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>445</v>
+      </c>
+      <c r="B95">
+        <v>-37</v>
+      </c>
+      <c r="C95">
+        <v>3</v>
+      </c>
+      <c r="D95" s="1">
+        <v>42800</v>
+      </c>
+      <c r="E95" t="s">
+        <v>81</v>
+      </c>
+      <c r="F95" t="s">
+        <v>446</v>
+      </c>
+      <c r="G95" t="s">
+        <v>125</v>
+      </c>
+      <c r="H95" s="2">
+        <v>49.99</v>
+      </c>
+      <c r="I95">
+        <v>2955</v>
+      </c>
+      <c r="J95">
+        <v>75605</v>
+      </c>
+      <c r="K95" t="s">
+        <v>447</v>
+      </c>
+      <c r="L95" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>449</v>
+      </c>
+      <c r="B96">
+        <v>-35</v>
+      </c>
+      <c r="C96">
+        <v>3</v>
+      </c>
+      <c r="D96" s="1">
+        <v>43017</v>
+      </c>
+      <c r="E96" t="s">
+        <v>87</v>
+      </c>
+      <c r="F96" t="s">
+        <v>450</v>
+      </c>
+      <c r="G96" t="s">
+        <v>442</v>
+      </c>
+      <c r="H96" t="s">
+        <v>451</v>
+      </c>
+      <c r="I96">
+        <v>1812</v>
+      </c>
+      <c r="J96">
+        <v>74303</v>
+      </c>
+      <c r="K96" t="s">
+        <v>452</v>
+      </c>
+      <c r="L96" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>454</v>
+      </c>
+      <c r="B97" t="s">
+        <v>48</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97" s="1">
+        <v>45498</v>
+      </c>
+      <c r="E97" t="s">
+        <v>123</v>
+      </c>
+      <c r="F97" t="s">
+        <v>455</v>
+      </c>
+      <c r="G97" t="s">
+        <v>456</v>
+      </c>
+      <c r="H97" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I97">
+        <v>1237</v>
+      </c>
+      <c r="K97" t="s">
+        <v>457</v>
+      </c>
+      <c r="L97" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>459</v>
+      </c>
+      <c r="B98" t="s">
+        <v>117</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98" s="1">
+        <v>45216</v>
+      </c>
+      <c r="E98" t="s">
+        <v>37</v>
+      </c>
+      <c r="F98" t="s">
+        <v>152</v>
+      </c>
+      <c r="G98" t="s">
+        <v>152</v>
+      </c>
+      <c r="H98" s="2">
+        <v>49.99</v>
+      </c>
+      <c r="I98">
+        <v>943</v>
+      </c>
+      <c r="J98">
+        <v>20463</v>
+      </c>
+      <c r="K98" t="s">
+        <v>460</v>
+      </c>
+      <c r="L98" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>462</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <v>2</v>
+      </c>
+      <c r="D99" s="1">
+        <v>45447</v>
+      </c>
+      <c r="E99" t="s">
+        <v>42</v>
+      </c>
+      <c r="F99" t="s">
+        <v>77</v>
+      </c>
+      <c r="G99" t="s">
+        <v>77</v>
+      </c>
+      <c r="H99" s="2">
+        <v>49.99</v>
+      </c>
+      <c r="I99">
+        <v>223</v>
+      </c>
+      <c r="J99">
+        <v>5024</v>
+      </c>
+      <c r="L99" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>464</v>
+      </c>
+      <c r="B100" t="s">
+        <v>117</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100" s="1">
+        <v>44855</v>
+      </c>
+      <c r="E100" t="s">
+        <v>72</v>
+      </c>
+      <c r="F100" t="s">
+        <v>351</v>
+      </c>
+      <c r="G100" t="s">
+        <v>277</v>
+      </c>
+      <c r="H100" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="I100">
+        <v>2044</v>
+      </c>
+      <c r="J100">
+        <v>50600</v>
+      </c>
+      <c r="K100" t="s">
+        <v>465</v>
+      </c>
+      <c r="L100" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>467</v>
+      </c>
+      <c r="B101" t="s">
+        <v>117</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101" s="1">
+        <v>43123</v>
+      </c>
+      <c r="E101" t="s">
+        <v>468</v>
+      </c>
+      <c r="F101" t="s">
+        <v>469</v>
+      </c>
+      <c r="G101" t="s">
+        <v>469</v>
+      </c>
+      <c r="H101" s="2">
+        <v>29.99</v>
+      </c>
+      <c r="I101">
+        <v>4797</v>
+      </c>
+      <c r="J101">
+        <v>250829</v>
+      </c>
+      <c r="K101" t="s">
+        <v>470</v>
+      </c>
+      <c r="L101" t="s">
+        <v>471</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC291C4-96D0-D14C-9991-8EE742F649AB}">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -5844,7 +9650,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD458E3F-9E53-804A-9E7D-8111A280BFC8}">
   <dimension ref="A1:L101"/>
   <sheetViews>

</xml_diff>

<commit_message>
1st of the month sept
</commit_message>
<xml_diff>
--- a/data/total_steam_titles.xlsx
+++ b/data/total_steam_titles.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenwang/Desktop/Makers/Steam_Roblox_Streamlit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AD42F8-815F-1546-B9A3-CDEC73C5924E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342F9C07-5E30-374E-B23C-9B998F80EDE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1240" windowWidth="24960" windowHeight="16760" xr2:uid="{91033176-3A50-8A43-8B19-6289EA40BB69}"/>
+    <workbookView xWindow="10340" yWindow="1360" windowWidth="24960" windowHeight="16760" xr2:uid="{91033176-3A50-8A43-8B19-6289EA40BB69}"/>
   </bookViews>
   <sheets>
-    <sheet name="2024-08-26" sheetId="8" r:id="rId1"/>
-    <sheet name="2024-08-19" sheetId="7" r:id="rId2"/>
-    <sheet name="2024-08-12" sheetId="6" r:id="rId3"/>
-    <sheet name="2024-08-05" sheetId="5" r:id="rId4"/>
-    <sheet name="2024-07-29" sheetId="4" r:id="rId5"/>
-    <sheet name="2024-07-23" sheetId="3" r:id="rId6"/>
-    <sheet name="2024-07-18" sheetId="1" r:id="rId7"/>
-    <sheet name="2024-07-11" sheetId="2" r:id="rId8"/>
+    <sheet name="2024-09-03" sheetId="9" r:id="rId1"/>
+    <sheet name="2024-08-26" sheetId="8" r:id="rId2"/>
+    <sheet name="2024-08-19" sheetId="7" r:id="rId3"/>
+    <sheet name="2024-08-12" sheetId="6" r:id="rId4"/>
+    <sheet name="2024-08-05" sheetId="5" r:id="rId5"/>
+    <sheet name="2024-07-29" sheetId="4" r:id="rId6"/>
+    <sheet name="2024-07-23" sheetId="3" r:id="rId7"/>
+    <sheet name="2024-07-18" sheetId="1" r:id="rId8"/>
+    <sheet name="2024-07-11" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5143" uniqueCount="1095">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5785" uniqueCount="1219">
   <si>
     <t>Game</t>
   </si>
@@ -3331,6 +3332,380 @@
   </si>
   <si>
     <t>https://store.steampowered.com/app/1222680/Need_for_Speed_Heat?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>Risk of Rain 2</t>
+  </si>
+  <si>
+    <t>Hopoo Games</t>
+  </si>
+  <si>
+    <t>Gearbox Publishing</t>
+  </si>
+  <si>
+    <t>Escape a chaotic alien planet by fighting through hordes of frenzied monsters ‚Äì with your friends, or on your own. Combine loot in surprising ways and master each character until you become the havoc you feared upon your first crash landing.</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/632360/Risk_of_Rain_2?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>Risk of Rain 2: Seekers of the Storm</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/2306620/Risk_of_Rain_2_Seekers_of_the_Storm?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>GUNDAM BREAKER 4</t>
+  </si>
+  <si>
+    <t>CRAFTS ÔºÜ MEISTER Co., Ltd</t>
+  </si>
+  <si>
+    <t>Create your own ultimate Gundam in the newest Gundam Breaker! With more customizable parts than ever before, you finally have the freedom to build your perfect Gunpla. Test it in battle using the brand new dual-weapon system and break parts off of your enemies and add them to your collection.</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/1672500/GUNDAM_BREAKER_4?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>SMITE 2</t>
+  </si>
+  <si>
+    <t>Action, Adventure, Casual, Massively Multiplayer, RPG, Strategy, Early Access</t>
+  </si>
+  <si>
+    <t>Titan Forge Games</t>
+  </si>
+  <si>
+    <t>Hi-Rez Studios</t>
+  </si>
+  <si>
+    <t>Become a god and wage war in SMITE 2, the Unreal Engine 5-powered sequel to the legendary third-person MOBA. Join our 24/7 Closed Alpha, where we are forging a challenging, team-based, mythological Battleground. Become a Founder today to jump into the action and be a part of the development.</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/2437170/SMITE_2?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>The Lord of the Rings: Return to Moria‚Ñ¢</t>
+  </si>
+  <si>
+    <t>Free Range Games</t>
+  </si>
+  <si>
+    <t>North Beach Games</t>
+  </si>
+  <si>
+    <t>The only survival crafting video game set in the Fourth Age of Middle-earth‚Ñ¢</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/2933130/The_Lord_of_the_Rings_Return_to_Moria?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>Visions of Mana</t>
+  </si>
+  <si>
+    <t>Explore a world of elemental spirits and adventure in the latest Mana action-RPG.</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/2490990/Visions_of_Mana?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>Core Keeper</t>
+  </si>
+  <si>
+    <t>Adventure, Casual, Indie, RPG</t>
+  </si>
+  <si>
+    <t>Pugstorm</t>
+  </si>
+  <si>
+    <t>Fireshine Games</t>
+  </si>
+  <si>
+    <t>Explore a vast cavern of creatures, relics and resources in a mining sandbox adventure for 1-8 players. Mine, build, fight, craft and farm to unravel the mystery of the ancient Core.</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/1621690/Core_Keeper?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>Squirrel with a Gun</t>
+  </si>
+  <si>
+    <t>Dee Dee Creations LLC</t>
+  </si>
+  <si>
+    <t>Maximum Entertainment</t>
+  </si>
+  <si>
+    <t>Squirrel, meet gun. As the neighborhood‚Äôs most obnoxious rodent, develop a knack (and a love?) for crime and mayhem in pursuit of golden acorns in this nutty sandbox shooter and puzzle platformer. Fight tooth, claw, and gun to escape a secret underground facility and defeat the Agents.</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/2067050/Squirrel_with_a_Gun?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>CarX Street</t>
+  </si>
+  <si>
+    <t>CarX Technologies, LLC</t>
+  </si>
+  <si>
+    <t>Conquer mountain roads, highways, and city streets. Build your dream car with detailed tuning that unleashes the potential of ‚ÄúCarX Technology‚Äù¬© physics. Take part in thrilling races, enjoying realistic gameplay and dynamic driving.</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/1114150/CarX_Street?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>Castlevania Dominus Collection</t>
+  </si>
+  <si>
+    <t>Three incredible action adventure games from the Castlevania series have finally returned, for the first time! But wait, there's more! Haunted Castle Revisited, a redesigned version of the very first Castlevania arcade game, makes its debut!</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/2369900/Castlevania_Dominus_Collection?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>Dead by Daylight - Castlevania Chapter</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/3103150/Dead_by_Daylight__Castlevania_Chapter?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>Kingdom Come: Deliverance</t>
+  </si>
+  <si>
+    <t>Warhorse Studios</t>
+  </si>
+  <si>
+    <t>Story-driven open-world RPG that immerses you in an epic adventure in the Holy Roman Empire. Avenge your parents' death as you battle invading forces, go on game-changing quests, and make influential choices. Explore castles, forests, villages and other realistic settings in medieval Bohemia!</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/379430/Kingdom_Come_Deliverance?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>LOCKDOWN Protocol</t>
+  </si>
+  <si>
+    <t>Action, Casual, Indie, Strategy, Early Access</t>
+  </si>
+  <si>
+    <t>Mirage Creative Lab</t>
+  </si>
+  <si>
+    <t>A first person social deduction game, combining real time action and communication, 3 to 8 players. While most players will do their best to complete objectives and ensure victory, a small portion of dissidents will try to stop them at all costs, without getting caught.</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/2780980/LOCKDOWN_Protocol?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>Tactical Breach Wizards</t>
+  </si>
+  <si>
+    <t>Suspicious Developments Inc</t>
+  </si>
+  <si>
+    <t>Suspicious Developments</t>
+  </si>
+  <si>
+    <t>In Tactical Breach Wizards, you lead a team of renegade wizards in kevlar through turn-based battles to unravel a modern conspiracy plot. Combine their unique spells in clever ways, or rewind time to try every crazy plan you can think of to punch a Traffic Warlock through a 4th story window.</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/1043810/Tactical_Breach_Wizards?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>NBA 2K25</t>
+  </si>
+  <si>
+    <t>Early Tip-Off | Hit the Court September 4th Command every court with authenticity and realism Powered by ProPLAY‚Ñ¢, giving you ultimate control over how you play in NBA 2K25. Define your legacy in MyCAREER, MyTEAM, MyNBA, and The W.</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/2878980/NBA_2K25?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>MARVEL vs. CAPCOM Fighting Collection: Arcade Classics</t>
+  </si>
+  <si>
+    <t>The legendary crossover hits are back! The action-packed lineup consisting of seven unique titles, is full of heavy hitters like X-MEN VS. STREET FIGHTER, and MARVEL vs. CAPCOM 2 New Age of Heroes. The collection also includes the rare beat 'em up game, THE PUNISHER.</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/2634890/MARVEL_vs_CAPCOM_Fighting_Collection_Arcade_Classics?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>Sid Meier's Civilization¬Æ VII</t>
+  </si>
+  <si>
+    <t>Firaxis Games</t>
+  </si>
+  <si>
+    <t>The award-winning strategy game franchise returns with a revolutionary new chapter. Sid Meier's Civilization¬Æ VII empowers you to build the greatest empire the world has ever known!</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/1295660/Sid_Meiers_Civilization_VII?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>Risk of Rain 2: Survivors of the Void</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/1607890/Risk_of_Rain_2_Survivors_of_the_Void?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>FINAL FANTASY XVI</t>
+  </si>
+  <si>
+    <t>An epic dark fantasy where fates are decided by mighty Eikons and the Dominants who wield them. This is the tale of Clive Rosfield, a tragic warrior who swears revenge on the Dark Eikon Ifrit, a mysterious entity that leaves naught but calamity in its wake.</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/2515020/FINAL_FANTASY_XVI?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>DRAGON BALL: Sparking! ZERO</t>
+  </si>
+  <si>
+    <t>Spike Chunsoft Co., Ltd.</t>
+  </si>
+  <si>
+    <t>DRAGON BALL: Sparking! ZERO takes the legendary gameplay of the Budokai Tenkaichi series and raises it to whole new levels. Make yours the destructive power of the strongest fighters ever to appear in DRAGON BALL!</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/1790600/DRAGON_BALL_Sparking_ZERO?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>MEMORIAPOLIS</t>
+  </si>
+  <si>
+    <t>5PM Studio</t>
+  </si>
+  <si>
+    <t>Memoriapolis invites you to construct a city that spans 2,500 years of history, from Antiquity to the Age of Enlightenment. Choose your culture, manage resources, face historical events, build "Wonders" to achieve the status of Capital of Capitals and leave your mark in history!</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/2228280/MEMORIAPOLIS?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>The Casting of Frank Stone‚Ñ¢</t>
+  </si>
+  <si>
+    <t>Supermassive Games</t>
+  </si>
+  <si>
+    <t>The shadow of Frank Stone looms over Cedar Hills, a town forever altered by his violent past. As a group of young friends are about to discover, Stone‚Äôs blood-soaked legacy cuts deep, leaving scars across families, generations, and the very fabric of reality itself.</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/2223840/The_Casting_of_Frank_Stone?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>Tales of Arise</t>
+  </si>
+  <si>
+    <t>300 years of tyranny. A mysterious mask. Lost pain and memories. Wield the Blazing Sword and join a mysterious, untouchable girl to fight your oppressors. Experience a tale of liberation, featuring characters with next-gen graphical expressiveness!</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/740130/Tales_of_Arise?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>Palia</t>
+  </si>
+  <si>
+    <t>Adventure, Casual, Indie, RPG, Simulation, Free To Play</t>
+  </si>
+  <si>
+    <t>Singularity 6 Corporation</t>
+  </si>
+  <si>
+    <t>Palia is a vibrant new world made just for you. Craft, cook, fish, and farm with friends as you live the life of your dreams and discover an enchanting adventure filled with colorful characters and a mystery to unravel.</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/2707930/Palia?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>Wartales</t>
+  </si>
+  <si>
+    <t>Shiro Games</t>
+  </si>
+  <si>
+    <t>Wartales is an open world RPG in which you lead a group of mercenaries in their search for wealth across a massive medieval universe. Explore the world, recruit companions, collect bounties and unravel the secrets of the tombs of the ancients!</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/1527950/Wartales?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>CarX Street - Deluxe Cars</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/3028020/CarX_Street__Deluxe_Cars?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>Aeons Echo
+(hidden by your preferences)</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/2832330/Aeons_Echo?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>Dying Light</t>
+  </si>
+  <si>
+    <t>First-person action survival game set in a post-apocalyptic open world overrun by flesh-hungry zombies. Roam a city devastated by a mysterious virus epidemic. Scavenge for supplies, craft weapons, and face hordes of the infected.</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/239140/Dying_Light?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>Harry Potter: Quidditch Champions</t>
+  </si>
+  <si>
+    <t>Action, Sports</t>
+  </si>
+  <si>
+    <t>Unbroken Studios</t>
+  </si>
+  <si>
+    <t>Your next chapter takes flight! Immerse yourself in the enchanting world of Quidditch by playing solo or sharing the magic with friends and family.</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/2878600/Harry_Potter_Quidditch_Champions?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>Disney Dreamlight Valley</t>
+  </si>
+  <si>
+    <t>Action, Adventure, Casual, RPG, Simulation</t>
+  </si>
+  <si>
+    <t>Gameloft</t>
+  </si>
+  <si>
+    <t>Explore a world filled with the magic of Disney as you discover rich stories and build the perfect neighborhood alongside Disney and Pixar heroes and villains in this new life-sim adventure game. Welcome to Disney Dreamlight Valley.</t>
+  </si>
+  <si>
+    <t>https://store.steampowered.com/app/1401590/Disney_Dreamlight_Valley?snr=1_7001_7002__7003</t>
+  </si>
+  <si>
+    <t>(MahjongSoul)
+(not available in your region)</t>
+  </si>
+  <si>
+    <t>Indie</t>
+  </si>
+  <si>
+    <t>Indie Budget Dev</t>
+  </si>
+  <si>
+    <t>~$2M</t>
+  </si>
+  <si>
+    <t>~&gt;$100K</t>
+  </si>
+  <si>
+    <t>~$36M</t>
+  </si>
+  <si>
+    <t>~$5M</t>
+  </si>
+  <si>
+    <t>~$1M</t>
+  </si>
+  <si>
+    <t>~$75K</t>
   </si>
 </sst>
 </file>
@@ -3724,10 +4099,3950 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42527168-848D-F84A-9A91-2353902B0E13}">
+  <dimension ref="A1:N101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1212</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>577</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45590</v>
+      </c>
+      <c r="G2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" t="s">
+        <v>578</v>
+      </c>
+      <c r="I2" t="s">
+        <v>187</v>
+      </c>
+      <c r="J2" s="2">
+        <v>69.989999999999995</v>
+      </c>
+      <c r="M2" t="s">
+        <v>579</v>
+      </c>
+      <c r="N2" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>-1</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>45523</v>
+      </c>
+      <c r="G3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="K3">
+        <v>538669</v>
+      </c>
+      <c r="M3" t="s">
+        <v>89</v>
+      </c>
+      <c r="N3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>770</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>45544</v>
+      </c>
+      <c r="G4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" t="s">
+        <v>771</v>
+      </c>
+      <c r="I4" t="s">
+        <v>772</v>
+      </c>
+      <c r="J4" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="M4" t="s">
+        <v>773</v>
+      </c>
+      <c r="N4" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>44054</v>
+      </c>
+      <c r="G5" t="s">
+        <v>315</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1096</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1097</v>
+      </c>
+      <c r="J5" s="2">
+        <v>24.99</v>
+      </c>
+      <c r="K5">
+        <v>6849</v>
+      </c>
+      <c r="L5">
+        <v>196384</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1098</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>45531</v>
+      </c>
+      <c r="G6" t="s">
+        <v>315</v>
+      </c>
+      <c r="H6" t="s">
+        <v>896</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1097</v>
+      </c>
+      <c r="J6" s="2">
+        <v>14.99</v>
+      </c>
+      <c r="K6">
+        <v>7666</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>-4</v>
+      </c>
+      <c r="E7">
+        <v>630</v>
+      </c>
+      <c r="F7" s="1">
+        <v>41142</v>
+      </c>
+      <c r="G7" t="s">
+        <v>700</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7">
+        <v>68648</v>
+      </c>
+      <c r="L7">
+        <v>8284052</v>
+      </c>
+      <c r="M7" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>-4</v>
+      </c>
+      <c r="E8">
+        <v>132</v>
+      </c>
+      <c r="N8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1">
+        <v>45473</v>
+      </c>
+      <c r="G9" t="s">
+        <v>702</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9">
+        <v>10656</v>
+      </c>
+      <c r="L9">
+        <v>83153</v>
+      </c>
+      <c r="M9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>-2</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1">
+        <v>45482</v>
+      </c>
+      <c r="G10" t="s">
+        <v>705</v>
+      </c>
+      <c r="H10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10">
+        <v>21301</v>
+      </c>
+      <c r="L10">
+        <v>82078</v>
+      </c>
+      <c r="M10" t="s">
+        <v>51</v>
+      </c>
+      <c r="N10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>382</v>
+      </c>
+      <c r="F11" s="1">
+        <v>42535</v>
+      </c>
+      <c r="G11" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I11" t="s">
+        <v>148</v>
+      </c>
+      <c r="J11" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="K11">
+        <v>5841</v>
+      </c>
+      <c r="L11">
+        <v>538348</v>
+      </c>
+      <c r="M11" t="s">
+        <v>149</v>
+      </c>
+      <c r="N11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>44967</v>
+      </c>
+      <c r="G12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" t="s">
+        <v>169</v>
+      </c>
+      <c r="I12" t="s">
+        <v>170</v>
+      </c>
+      <c r="J12" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="K12">
+        <v>2590</v>
+      </c>
+      <c r="L12">
+        <v>200091</v>
+      </c>
+      <c r="M12" t="s">
+        <v>171</v>
+      </c>
+      <c r="N12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>-7</v>
+      </c>
+      <c r="E13">
+        <v>597</v>
+      </c>
+      <c r="F13" s="1">
+        <v>41358</v>
+      </c>
+      <c r="G13" t="s">
+        <v>707</v>
+      </c>
+      <c r="H13" t="s">
+        <v>135</v>
+      </c>
+      <c r="I13" t="s">
+        <v>135</v>
+      </c>
+      <c r="J13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13">
+        <v>4546</v>
+      </c>
+      <c r="L13">
+        <v>589480</v>
+      </c>
+      <c r="M13" t="s">
+        <v>136</v>
+      </c>
+      <c r="N13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>51</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1">
+        <v>45532</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1103</v>
+      </c>
+      <c r="I14" t="s">
+        <v>308</v>
+      </c>
+      <c r="J14" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="K14">
+        <v>1443</v>
+      </c>
+      <c r="M14" t="s">
+        <v>1104</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>29</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>45531</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1107</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1108</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1109</v>
+      </c>
+      <c r="J15" s="2">
+        <v>29.99</v>
+      </c>
+      <c r="K15">
+        <v>1445</v>
+      </c>
+      <c r="M15" t="s">
+        <v>1110</v>
+      </c>
+      <c r="N15" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>302</v>
+      </c>
+      <c r="B16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>45</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>45539</v>
+      </c>
+      <c r="G16" t="s">
+        <v>196</v>
+      </c>
+      <c r="H16" t="s">
+        <v>303</v>
+      </c>
+      <c r="I16" t="s">
+        <v>103</v>
+      </c>
+      <c r="J16" s="2">
+        <v>29.99</v>
+      </c>
+      <c r="K16">
+        <v>3458</v>
+      </c>
+      <c r="M16" t="s">
+        <v>304</v>
+      </c>
+      <c r="N16" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>-6</v>
+      </c>
+      <c r="E17">
+        <v>375</v>
+      </c>
+      <c r="F17" s="1">
+        <v>41501</v>
+      </c>
+      <c r="G17" t="s">
+        <v>710</v>
+      </c>
+      <c r="H17" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17">
+        <v>11315</v>
+      </c>
+      <c r="L17">
+        <v>531412</v>
+      </c>
+      <c r="M17" t="s">
+        <v>98</v>
+      </c>
+      <c r="N17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>-4</v>
+      </c>
+      <c r="E18">
+        <v>90</v>
+      </c>
+      <c r="F18" s="1">
+        <v>45141</v>
+      </c>
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" t="s">
+        <v>55</v>
+      </c>
+      <c r="J18" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="K18">
+        <v>9694</v>
+      </c>
+      <c r="L18">
+        <v>574358</v>
+      </c>
+      <c r="M18" t="s">
+        <v>56</v>
+      </c>
+      <c r="N18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>45531</v>
+      </c>
+      <c r="G19" t="s">
+        <v>572</v>
+      </c>
+      <c r="H19" t="s">
+        <v>1113</v>
+      </c>
+      <c r="I19" t="s">
+        <v>1114</v>
+      </c>
+      <c r="J19" s="2">
+        <v>24.99</v>
+      </c>
+      <c r="K19">
+        <v>920</v>
+      </c>
+      <c r="M19" t="s">
+        <v>1115</v>
+      </c>
+      <c r="N19" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B20" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>45533</v>
+      </c>
+      <c r="G20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" t="s">
+        <v>157</v>
+      </c>
+      <c r="I20" t="s">
+        <v>157</v>
+      </c>
+      <c r="J20" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="K20">
+        <v>568</v>
+      </c>
+      <c r="M20" t="s">
+        <v>1118</v>
+      </c>
+      <c r="N20" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>43</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21" s="1">
+        <v>45531</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H21" t="s">
+        <v>1122</v>
+      </c>
+      <c r="I21" t="s">
+        <v>1123</v>
+      </c>
+      <c r="J21" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="K21">
+        <v>1866</v>
+      </c>
+      <c r="L21">
+        <v>27405</v>
+      </c>
+      <c r="M21" t="s">
+        <v>1124</v>
+      </c>
+      <c r="N21" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>45533</v>
+      </c>
+      <c r="G22" t="s">
+        <v>227</v>
+      </c>
+      <c r="H22" t="s">
+        <v>1127</v>
+      </c>
+      <c r="I22" t="s">
+        <v>1128</v>
+      </c>
+      <c r="J22" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="K22">
+        <v>825</v>
+      </c>
+      <c r="M22" t="s">
+        <v>1129</v>
+      </c>
+      <c r="N22" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>-8</v>
+      </c>
+      <c r="E23">
+        <v>40</v>
+      </c>
+      <c r="F23" s="1">
+        <v>44616</v>
+      </c>
+      <c r="G23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" t="s">
+        <v>547</v>
+      </c>
+      <c r="I23" t="s">
+        <v>547</v>
+      </c>
+      <c r="J23" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="K23">
+        <v>13343</v>
+      </c>
+      <c r="L23">
+        <v>700154</v>
+      </c>
+      <c r="M23" t="s">
+        <v>39</v>
+      </c>
+      <c r="N23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>55</v>
+      </c>
+      <c r="E24">
+        <v>26</v>
+      </c>
+      <c r="F24" s="1">
+        <v>43804</v>
+      </c>
+      <c r="G24" t="s">
+        <v>81</v>
+      </c>
+      <c r="H24" t="s">
+        <v>83</v>
+      </c>
+      <c r="I24" t="s">
+        <v>83</v>
+      </c>
+      <c r="J24" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="K24">
+        <v>10807</v>
+      </c>
+      <c r="L24">
+        <v>564739</v>
+      </c>
+      <c r="M24" t="s">
+        <v>92</v>
+      </c>
+      <c r="N24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>155</v>
+      </c>
+      <c r="B25" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>405</v>
+      </c>
+      <c r="F25" s="1">
+        <v>41688</v>
+      </c>
+      <c r="G25" t="s">
+        <v>156</v>
+      </c>
+      <c r="H25" t="s">
+        <v>157</v>
+      </c>
+      <c r="I25" t="s">
+        <v>157</v>
+      </c>
+      <c r="J25" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="K25">
+        <v>629</v>
+      </c>
+      <c r="L25">
+        <v>70118</v>
+      </c>
+      <c r="M25" t="s">
+        <v>158</v>
+      </c>
+      <c r="N25" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>459</v>
+      </c>
+      <c r="B26" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>-8</v>
+      </c>
+      <c r="E26">
+        <v>7</v>
+      </c>
+      <c r="F26" s="1">
+        <v>45216</v>
+      </c>
+      <c r="G26" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" t="s">
+        <v>152</v>
+      </c>
+      <c r="I26" t="s">
+        <v>152</v>
+      </c>
+      <c r="J26" s="2">
+        <v>49.99</v>
+      </c>
+      <c r="K26">
+        <v>1939</v>
+      </c>
+      <c r="L26">
+        <v>22511</v>
+      </c>
+      <c r="M26" t="s">
+        <v>460</v>
+      </c>
+      <c r="N26" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>45533</v>
+      </c>
+      <c r="G27" t="s">
+        <v>649</v>
+      </c>
+      <c r="H27" t="s">
+        <v>1132</v>
+      </c>
+      <c r="I27" t="s">
+        <v>1132</v>
+      </c>
+      <c r="J27" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="K27">
+        <v>3066</v>
+      </c>
+      <c r="M27" t="s">
+        <v>1133</v>
+      </c>
+      <c r="N27" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>-5</v>
+      </c>
+      <c r="E28">
+        <v>459</v>
+      </c>
+      <c r="F28" s="1">
+        <v>42339</v>
+      </c>
+      <c r="G28" t="s">
+        <v>123</v>
+      </c>
+      <c r="H28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I28" t="s">
+        <v>125</v>
+      </c>
+      <c r="J28" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="K28">
+        <v>7891</v>
+      </c>
+      <c r="L28">
+        <v>1116776</v>
+      </c>
+      <c r="M28" t="s">
+        <v>126</v>
+      </c>
+      <c r="N28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>-13</v>
+      </c>
+      <c r="E29">
+        <v>11</v>
+      </c>
+      <c r="F29" s="1">
+        <v>45148</v>
+      </c>
+      <c r="G29" t="s">
+        <v>700</v>
+      </c>
+      <c r="H29" t="s">
+        <v>152</v>
+      </c>
+      <c r="I29" t="s">
+        <v>152</v>
+      </c>
+      <c r="J29" t="s">
+        <v>27</v>
+      </c>
+      <c r="K29">
+        <v>9258</v>
+      </c>
+      <c r="L29">
+        <v>293822</v>
+      </c>
+      <c r="M29" t="s">
+        <v>153</v>
+      </c>
+      <c r="N29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <v>45531</v>
+      </c>
+      <c r="G30" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" t="s">
+        <v>119</v>
+      </c>
+      <c r="I30" t="s">
+        <v>119</v>
+      </c>
+      <c r="J30" s="2">
+        <v>24.99</v>
+      </c>
+      <c r="K30">
+        <v>519</v>
+      </c>
+      <c r="M30" t="s">
+        <v>1136</v>
+      </c>
+      <c r="N30" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1">
+        <v>45531</v>
+      </c>
+      <c r="G31" t="s">
+        <v>123</v>
+      </c>
+      <c r="H31" t="s">
+        <v>148</v>
+      </c>
+      <c r="I31" t="s">
+        <v>148</v>
+      </c>
+      <c r="J31" s="2">
+        <v>7.99</v>
+      </c>
+      <c r="K31">
+        <v>301</v>
+      </c>
+      <c r="N31" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>472</v>
+      </c>
+      <c r="B32" t="b">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>48</v>
+      </c>
+      <c r="E32">
+        <v>7</v>
+      </c>
+      <c r="F32" s="1">
+        <v>41130</v>
+      </c>
+      <c r="G32" t="s">
+        <v>855</v>
+      </c>
+      <c r="H32" t="s">
+        <v>474</v>
+      </c>
+      <c r="I32" t="s">
+        <v>475</v>
+      </c>
+      <c r="J32" t="s">
+        <v>15</v>
+      </c>
+      <c r="K32">
+        <v>102</v>
+      </c>
+      <c r="L32">
+        <v>13014</v>
+      </c>
+      <c r="M32" t="s">
+        <v>476</v>
+      </c>
+      <c r="N32" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" t="b">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>43</v>
+      </c>
+      <c r="F33" s="1">
+        <v>43739</v>
+      </c>
+      <c r="G33" t="s">
+        <v>704</v>
+      </c>
+      <c r="H33" t="s">
+        <v>77</v>
+      </c>
+      <c r="I33" t="s">
+        <v>77</v>
+      </c>
+      <c r="J33" t="s">
+        <v>27</v>
+      </c>
+      <c r="K33">
+        <v>3188</v>
+      </c>
+      <c r="L33">
+        <v>610914</v>
+      </c>
+      <c r="M33" t="s">
+        <v>78</v>
+      </c>
+      <c r="N33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1">
+        <v>43144</v>
+      </c>
+      <c r="G34" t="s">
+        <v>87</v>
+      </c>
+      <c r="H34" t="s">
+        <v>1141</v>
+      </c>
+      <c r="I34" t="s">
+        <v>1141</v>
+      </c>
+      <c r="J34" s="2">
+        <v>29.99</v>
+      </c>
+      <c r="K34">
+        <v>2153</v>
+      </c>
+      <c r="L34">
+        <v>100029</v>
+      </c>
+      <c r="M34" t="s">
+        <v>1142</v>
+      </c>
+      <c r="N34" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>-16</v>
+      </c>
+      <c r="E35">
+        <v>200</v>
+      </c>
+      <c r="F35" s="1">
+        <v>44139</v>
+      </c>
+      <c r="G35" t="s">
+        <v>704</v>
+      </c>
+      <c r="H35" t="s">
+        <v>43</v>
+      </c>
+      <c r="I35" t="s">
+        <v>44</v>
+      </c>
+      <c r="J35" t="s">
+        <v>27</v>
+      </c>
+      <c r="K35">
+        <v>16410</v>
+      </c>
+      <c r="L35">
+        <v>942662</v>
+      </c>
+      <c r="M35" t="s">
+        <v>45</v>
+      </c>
+      <c r="N35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B36" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>-14</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36" s="1">
+        <v>45495</v>
+      </c>
+      <c r="G36" t="s">
+        <v>1145</v>
+      </c>
+      <c r="H36" t="s">
+        <v>1146</v>
+      </c>
+      <c r="I36" t="s">
+        <v>1146</v>
+      </c>
+      <c r="J36" s="2">
+        <v>9.99</v>
+      </c>
+      <c r="K36">
+        <v>1733</v>
+      </c>
+      <c r="L36">
+        <v>1795</v>
+      </c>
+      <c r="M36" t="s">
+        <v>1147</v>
+      </c>
+      <c r="N36" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B37" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>-16</v>
+      </c>
+      <c r="E37">
+        <v>4</v>
+      </c>
+      <c r="F37" s="1">
+        <v>45519</v>
+      </c>
+      <c r="G37" t="s">
+        <v>1016</v>
+      </c>
+      <c r="H37" t="s">
+        <v>1017</v>
+      </c>
+      <c r="I37" t="s">
+        <v>44</v>
+      </c>
+      <c r="J37" s="2">
+        <v>69.989999999999995</v>
+      </c>
+      <c r="K37">
+        <v>576</v>
+      </c>
+      <c r="M37" t="s">
+        <v>1018</v>
+      </c>
+      <c r="N37" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>220</v>
+      </c>
+      <c r="B38" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>-9</v>
+      </c>
+      <c r="E38">
+        <v>139</v>
+      </c>
+      <c r="F38" s="1">
+        <v>44603</v>
+      </c>
+      <c r="G38" t="s">
+        <v>736</v>
+      </c>
+      <c r="H38" t="s">
+        <v>222</v>
+      </c>
+      <c r="I38" t="s">
+        <v>223</v>
+      </c>
+      <c r="J38" t="s">
+        <v>27</v>
+      </c>
+      <c r="K38">
+        <v>496</v>
+      </c>
+      <c r="L38">
+        <v>200472</v>
+      </c>
+      <c r="M38" t="s">
+        <v>224</v>
+      </c>
+      <c r="N38" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>138</v>
+      </c>
+      <c r="B39" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>-4</v>
+      </c>
+      <c r="E39">
+        <v>480</v>
+      </c>
+      <c r="F39" s="1">
+        <v>43139</v>
+      </c>
+      <c r="G39" t="s">
+        <v>139</v>
+      </c>
+      <c r="H39" t="s">
+        <v>140</v>
+      </c>
+      <c r="I39" t="s">
+        <v>140</v>
+      </c>
+      <c r="J39" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="K39">
+        <v>9692</v>
+      </c>
+      <c r="L39">
+        <v>909087</v>
+      </c>
+      <c r="M39" t="s">
+        <v>141</v>
+      </c>
+      <c r="N39" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" t="b">
+        <v>0</v>
+      </c>
+      <c r="D40" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1">
+        <v>45456</v>
+      </c>
+      <c r="G40" t="s">
+        <v>87</v>
+      </c>
+      <c r="H40" t="s">
+        <v>157</v>
+      </c>
+      <c r="I40" t="s">
+        <v>157</v>
+      </c>
+      <c r="J40" s="2">
+        <v>49.99</v>
+      </c>
+      <c r="K40">
+        <v>345</v>
+      </c>
+      <c r="L40">
+        <v>4191</v>
+      </c>
+      <c r="M40" t="s">
+        <v>178</v>
+      </c>
+      <c r="N40" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>201</v>
+      </c>
+      <c r="B41" t="b">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>-16</v>
+      </c>
+      <c r="E41">
+        <v>230</v>
+      </c>
+      <c r="F41" s="1">
+        <v>43935</v>
+      </c>
+      <c r="G41" t="s">
+        <v>72</v>
+      </c>
+      <c r="H41" t="s">
+        <v>202</v>
+      </c>
+      <c r="I41" t="s">
+        <v>203</v>
+      </c>
+      <c r="J41" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="K41">
+        <v>803</v>
+      </c>
+      <c r="L41">
+        <v>61151</v>
+      </c>
+      <c r="M41" t="s">
+        <v>204</v>
+      </c>
+      <c r="N41" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" t="b">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>-11</v>
+      </c>
+      <c r="E42">
+        <v>503</v>
+      </c>
+      <c r="F42" s="1">
+        <v>42108</v>
+      </c>
+      <c r="G42" t="s">
+        <v>81</v>
+      </c>
+      <c r="H42" t="s">
+        <v>82</v>
+      </c>
+      <c r="I42" t="s">
+        <v>83</v>
+      </c>
+      <c r="J42" s="2">
+        <v>39.979999999999997</v>
+      </c>
+      <c r="K42">
+        <v>20797</v>
+      </c>
+      <c r="L42">
+        <v>1701639</v>
+      </c>
+      <c r="M42" t="s">
+        <v>84</v>
+      </c>
+      <c r="N42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>185</v>
+      </c>
+      <c r="B43" t="b">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>-17</v>
+      </c>
+      <c r="E43">
+        <v>111</v>
+      </c>
+      <c r="F43" s="1">
+        <v>44862</v>
+      </c>
+      <c r="G43" t="s">
+        <v>123</v>
+      </c>
+      <c r="H43" t="s">
+        <v>186</v>
+      </c>
+      <c r="I43" t="s">
+        <v>187</v>
+      </c>
+      <c r="J43" s="2">
+        <v>69.989999999999995</v>
+      </c>
+      <c r="K43">
+        <v>6110</v>
+      </c>
+      <c r="L43">
+        <v>330318</v>
+      </c>
+      <c r="M43" t="s">
+        <v>188</v>
+      </c>
+      <c r="N43" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>311</v>
+      </c>
+      <c r="B44" t="b">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>-5</v>
+      </c>
+      <c r="E44">
+        <v>9</v>
+      </c>
+      <c r="F44" s="1">
+        <v>39365</v>
+      </c>
+      <c r="G44" t="s">
+        <v>700</v>
+      </c>
+      <c r="H44" t="s">
+        <v>20</v>
+      </c>
+      <c r="I44" t="s">
+        <v>20</v>
+      </c>
+      <c r="J44" t="s">
+        <v>27</v>
+      </c>
+      <c r="K44">
+        <v>7656</v>
+      </c>
+      <c r="L44">
+        <v>1116337</v>
+      </c>
+      <c r="M44" t="s">
+        <v>312</v>
+      </c>
+      <c r="N44" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" t="b">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>-28</v>
+      </c>
+      <c r="E45">
+        <v>9</v>
+      </c>
+      <c r="F45" s="1">
+        <v>41464</v>
+      </c>
+      <c r="G45" t="s">
+        <v>703</v>
+      </c>
+      <c r="H45" t="s">
+        <v>20</v>
+      </c>
+      <c r="I45" t="s">
+        <v>20</v>
+      </c>
+      <c r="J45" t="s">
+        <v>27</v>
+      </c>
+      <c r="K45">
+        <v>26718</v>
+      </c>
+      <c r="L45">
+        <v>2311554</v>
+      </c>
+      <c r="M45" t="s">
+        <v>21</v>
+      </c>
+      <c r="N45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>238</v>
+      </c>
+      <c r="B46" t="b">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>-13</v>
+      </c>
+      <c r="E46">
+        <v>502</v>
+      </c>
+      <c r="F46" s="1">
+        <v>41733</v>
+      </c>
+      <c r="G46" t="s">
+        <v>239</v>
+      </c>
+      <c r="H46" t="s">
+        <v>240</v>
+      </c>
+      <c r="I46" t="s">
+        <v>203</v>
+      </c>
+      <c r="J46" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="K46">
+        <v>712</v>
+      </c>
+      <c r="L46">
+        <v>122537</v>
+      </c>
+      <c r="M46" t="s">
+        <v>241</v>
+      </c>
+      <c r="N46" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>215</v>
+      </c>
+      <c r="B47" t="b">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>-13</v>
+      </c>
+      <c r="E47">
+        <v>34</v>
+      </c>
+      <c r="F47" s="1">
+        <v>45330</v>
+      </c>
+      <c r="G47" t="s">
+        <v>123</v>
+      </c>
+      <c r="H47" t="s">
+        <v>216</v>
+      </c>
+      <c r="I47" t="s">
+        <v>217</v>
+      </c>
+      <c r="J47" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="K47">
+        <v>12598</v>
+      </c>
+      <c r="L47">
+        <v>664641</v>
+      </c>
+      <c r="M47" t="s">
+        <v>218</v>
+      </c>
+      <c r="N47" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" t="b">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>16</v>
+      </c>
+      <c r="F48" s="1">
+        <v>43090</v>
+      </c>
+      <c r="G48" t="s">
+        <v>701</v>
+      </c>
+      <c r="H48" t="s">
+        <v>14</v>
+      </c>
+      <c r="I48" t="s">
+        <v>14</v>
+      </c>
+      <c r="J48" t="s">
+        <v>27</v>
+      </c>
+      <c r="K48">
+        <v>20934</v>
+      </c>
+      <c r="L48">
+        <v>2422565</v>
+      </c>
+      <c r="M48" t="s">
+        <v>16</v>
+      </c>
+      <c r="N48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>210</v>
+      </c>
+      <c r="B49" t="b">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>220</v>
+      </c>
+      <c r="F49" s="1">
+        <v>41884</v>
+      </c>
+      <c r="G49" t="s">
+        <v>721</v>
+      </c>
+      <c r="H49" t="s">
+        <v>212</v>
+      </c>
+      <c r="I49" t="s">
+        <v>44</v>
+      </c>
+      <c r="J49" t="s">
+        <v>27</v>
+      </c>
+      <c r="K49">
+        <v>3152</v>
+      </c>
+      <c r="L49">
+        <v>148283</v>
+      </c>
+      <c r="M49" t="s">
+        <v>213</v>
+      </c>
+      <c r="N49" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>992</v>
+      </c>
+      <c r="B50" t="b">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>-37</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="F50" s="1">
+        <v>45519</v>
+      </c>
+      <c r="G50" t="s">
+        <v>345</v>
+      </c>
+      <c r="H50" t="s">
+        <v>993</v>
+      </c>
+      <c r="I50" t="s">
+        <v>994</v>
+      </c>
+      <c r="J50" s="2">
+        <v>49.99</v>
+      </c>
+      <c r="K50">
+        <v>3484</v>
+      </c>
+      <c r="M50" t="s">
+        <v>995</v>
+      </c>
+      <c r="N50" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B51" t="b">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>-41</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51" s="1">
+        <v>45526</v>
+      </c>
+      <c r="G51" t="s">
+        <v>532</v>
+      </c>
+      <c r="H51" t="s">
+        <v>1150</v>
+      </c>
+      <c r="I51" t="s">
+        <v>1151</v>
+      </c>
+      <c r="J51" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="K51">
+        <v>3428</v>
+      </c>
+      <c r="M51" t="s">
+        <v>1152</v>
+      </c>
+      <c r="N51" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>589</v>
+      </c>
+      <c r="B52" t="b">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>8</v>
+      </c>
+      <c r="F52" s="1">
+        <v>45069</v>
+      </c>
+      <c r="G52" t="s">
+        <v>765</v>
+      </c>
+      <c r="H52" t="s">
+        <v>591</v>
+      </c>
+      <c r="I52" t="s">
+        <v>591</v>
+      </c>
+      <c r="J52" t="s">
+        <v>27</v>
+      </c>
+      <c r="K52">
+        <v>964</v>
+      </c>
+      <c r="L52">
+        <v>12922</v>
+      </c>
+      <c r="M52" t="s">
+        <v>592</v>
+      </c>
+      <c r="N52" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>288</v>
+      </c>
+      <c r="B53" t="b">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+      <c r="E53">
+        <v>142</v>
+      </c>
+      <c r="F53" s="1">
+        <v>45273</v>
+      </c>
+      <c r="G53" t="s">
+        <v>289</v>
+      </c>
+      <c r="H53" t="s">
+        <v>290</v>
+      </c>
+      <c r="I53" t="s">
+        <v>290</v>
+      </c>
+      <c r="J53" s="2">
+        <v>49.99</v>
+      </c>
+      <c r="K53">
+        <v>3194</v>
+      </c>
+      <c r="L53">
+        <v>149882</v>
+      </c>
+      <c r="M53" t="s">
+        <v>291</v>
+      </c>
+      <c r="N53" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>594</v>
+      </c>
+      <c r="B54" t="b">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>6</v>
+      </c>
+      <c r="E54">
+        <v>222</v>
+      </c>
+      <c r="J54" s="2">
+        <v>499</v>
+      </c>
+      <c r="N54" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" t="b">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>65</v>
+      </c>
+      <c r="F55" s="1">
+        <v>44174</v>
+      </c>
+      <c r="G55" t="s">
+        <v>72</v>
+      </c>
+      <c r="H55" t="s">
+        <v>73</v>
+      </c>
+      <c r="I55" t="s">
+        <v>73</v>
+      </c>
+      <c r="J55" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="K55">
+        <v>7314</v>
+      </c>
+      <c r="L55">
+        <v>676217</v>
+      </c>
+      <c r="M55" t="s">
+        <v>74</v>
+      </c>
+      <c r="N55" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>899</v>
+      </c>
+      <c r="B56" t="b">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>-18</v>
+      </c>
+      <c r="E56">
+        <v>5</v>
+      </c>
+      <c r="F56" s="1">
+        <v>45509</v>
+      </c>
+      <c r="G56" t="s">
+        <v>375</v>
+      </c>
+      <c r="H56" t="s">
+        <v>900</v>
+      </c>
+      <c r="I56" t="s">
+        <v>900</v>
+      </c>
+      <c r="J56" s="2">
+        <v>13.99</v>
+      </c>
+      <c r="K56">
+        <v>6664</v>
+      </c>
+      <c r="M56" t="s">
+        <v>901</v>
+      </c>
+      <c r="N56" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B57" t="b">
+        <v>0</v>
+      </c>
+      <c r="D57" t="s">
+        <v>48</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1">
+        <v>45541</v>
+      </c>
+      <c r="G57" t="s">
+        <v>107</v>
+      </c>
+      <c r="H57" t="s">
+        <v>674</v>
+      </c>
+      <c r="I57" t="s">
+        <v>198</v>
+      </c>
+      <c r="J57" s="2">
+        <v>69.989999999999995</v>
+      </c>
+      <c r="M57" t="s">
+        <v>1155</v>
+      </c>
+      <c r="N57" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>335</v>
+      </c>
+      <c r="B58" t="b">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>-18</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="F58" s="1">
+        <v>44595</v>
+      </c>
+      <c r="G58" t="s">
+        <v>87</v>
+      </c>
+      <c r="H58" t="s">
+        <v>336</v>
+      </c>
+      <c r="I58" t="s">
+        <v>336</v>
+      </c>
+      <c r="J58" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="K58">
+        <v>1707</v>
+      </c>
+      <c r="L58">
+        <v>131017</v>
+      </c>
+      <c r="M58" t="s">
+        <v>337</v>
+      </c>
+      <c r="N58" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>344</v>
+      </c>
+      <c r="B59" t="b">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>35</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+      <c r="F59" s="1">
+        <v>42527</v>
+      </c>
+      <c r="G59" t="s">
+        <v>345</v>
+      </c>
+      <c r="H59" t="s">
+        <v>346</v>
+      </c>
+      <c r="I59" t="s">
+        <v>347</v>
+      </c>
+      <c r="J59" s="2">
+        <v>49.99</v>
+      </c>
+      <c r="K59">
+        <v>3206</v>
+      </c>
+      <c r="L59">
+        <v>217077</v>
+      </c>
+      <c r="M59" t="s">
+        <v>348</v>
+      </c>
+      <c r="N59" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" t="b">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>-17</v>
+      </c>
+      <c r="E60">
+        <v>17</v>
+      </c>
+      <c r="F60" s="1">
+        <v>45463</v>
+      </c>
+      <c r="G60" t="s">
+        <v>37</v>
+      </c>
+      <c r="H60" t="s">
+        <v>547</v>
+      </c>
+      <c r="I60" t="s">
+        <v>547</v>
+      </c>
+      <c r="J60" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="K60">
+        <v>2171</v>
+      </c>
+      <c r="L60">
+        <v>78012</v>
+      </c>
+      <c r="N60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>600</v>
+      </c>
+      <c r="B61" t="b">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>-24</v>
+      </c>
+      <c r="E61">
+        <v>7</v>
+      </c>
+      <c r="F61" s="1">
+        <v>41570</v>
+      </c>
+      <c r="G61" t="s">
+        <v>706</v>
+      </c>
+      <c r="H61" t="s">
+        <v>602</v>
+      </c>
+      <c r="I61" t="s">
+        <v>602</v>
+      </c>
+      <c r="J61" t="s">
+        <v>27</v>
+      </c>
+      <c r="K61">
+        <v>2276</v>
+      </c>
+      <c r="L61">
+        <v>225617</v>
+      </c>
+      <c r="M61" t="s">
+        <v>603</v>
+      </c>
+      <c r="N61" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>694</v>
+      </c>
+      <c r="B62" t="b">
+        <v>0</v>
+      </c>
+      <c r="D62" t="s">
+        <v>117</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" s="1">
+        <v>45224</v>
+      </c>
+      <c r="G62" t="s">
+        <v>695</v>
+      </c>
+      <c r="H62" t="s">
+        <v>696</v>
+      </c>
+      <c r="I62" t="s">
+        <v>697</v>
+      </c>
+      <c r="J62" s="2">
+        <v>44.99</v>
+      </c>
+      <c r="K62">
+        <v>1296</v>
+      </c>
+      <c r="L62">
+        <v>53119</v>
+      </c>
+      <c r="M62" t="s">
+        <v>698</v>
+      </c>
+      <c r="N62" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>116</v>
+      </c>
+      <c r="B63" t="b">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>7</v>
+      </c>
+      <c r="E63">
+        <v>8</v>
+      </c>
+      <c r="F63" s="1">
+        <v>44579</v>
+      </c>
+      <c r="G63" t="s">
+        <v>766</v>
+      </c>
+      <c r="H63" t="s">
+        <v>119</v>
+      </c>
+      <c r="I63" t="s">
+        <v>119</v>
+      </c>
+      <c r="J63" t="s">
+        <v>27</v>
+      </c>
+      <c r="K63">
+        <v>1027</v>
+      </c>
+      <c r="L63">
+        <v>76320</v>
+      </c>
+      <c r="M63" t="s">
+        <v>120</v>
+      </c>
+      <c r="N63" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>195</v>
+      </c>
+      <c r="B64" t="b">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>-18</v>
+      </c>
+      <c r="E64">
+        <v>2</v>
+      </c>
+      <c r="F64" s="1">
+        <v>42663</v>
+      </c>
+      <c r="G64" t="s">
+        <v>196</v>
+      </c>
+      <c r="H64" t="s">
+        <v>197</v>
+      </c>
+      <c r="I64" t="s">
+        <v>198</v>
+      </c>
+      <c r="J64" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="K64">
+        <v>3458</v>
+      </c>
+      <c r="L64">
+        <v>236793</v>
+      </c>
+      <c r="M64" t="s">
+        <v>199</v>
+      </c>
+      <c r="N64" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>895</v>
+      </c>
+      <c r="B65" t="b">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>-37</v>
+      </c>
+      <c r="E65">
+        <v>4</v>
+      </c>
+      <c r="F65" s="1">
+        <v>43903</v>
+      </c>
+      <c r="G65" t="s">
+        <v>37</v>
+      </c>
+      <c r="H65" t="s">
+        <v>896</v>
+      </c>
+      <c r="I65" t="s">
+        <v>198</v>
+      </c>
+      <c r="J65" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="K65">
+        <v>2211</v>
+      </c>
+      <c r="L65">
+        <v>106696</v>
+      </c>
+      <c r="M65" t="s">
+        <v>897</v>
+      </c>
+      <c r="N65" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B66" t="b">
+        <v>0</v>
+      </c>
+      <c r="D66" t="s">
+        <v>48</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66" s="1">
+        <v>45546</v>
+      </c>
+      <c r="G66" t="s">
+        <v>123</v>
+      </c>
+      <c r="H66" t="s">
+        <v>264</v>
+      </c>
+      <c r="I66" t="s">
+        <v>264</v>
+      </c>
+      <c r="J66" s="2">
+        <v>49.99</v>
+      </c>
+      <c r="M66" t="s">
+        <v>1158</v>
+      </c>
+      <c r="N66" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B67" t="b">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>-35</v>
+      </c>
+      <c r="E67">
+        <v>3</v>
+      </c>
+      <c r="F67" s="1">
+        <v>43704</v>
+      </c>
+      <c r="G67" t="s">
+        <v>123</v>
+      </c>
+      <c r="H67" t="s">
+        <v>687</v>
+      </c>
+      <c r="I67" t="s">
+        <v>687</v>
+      </c>
+      <c r="J67" s="2">
+        <v>29.99</v>
+      </c>
+      <c r="K67">
+        <v>15967</v>
+      </c>
+      <c r="L67">
+        <v>177090</v>
+      </c>
+      <c r="M67" t="s">
+        <v>1013</v>
+      </c>
+      <c r="N67" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B68" t="b">
+        <v>0</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D68">
+        <v>-59</v>
+      </c>
+      <c r="E68">
+        <v>2</v>
+      </c>
+      <c r="F68" s="1">
+        <v>45699</v>
+      </c>
+      <c r="G68" t="s">
+        <v>345</v>
+      </c>
+      <c r="H68" t="s">
+        <v>1161</v>
+      </c>
+      <c r="I68" t="s">
+        <v>198</v>
+      </c>
+      <c r="J68" s="2">
+        <v>69.989999999999995</v>
+      </c>
+      <c r="M68" t="s">
+        <v>1162</v>
+      </c>
+      <c r="N68" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>365</v>
+      </c>
+      <c r="B69" t="b">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
+      <c r="E69">
+        <v>27</v>
+      </c>
+      <c r="F69" s="1">
+        <v>42314</v>
+      </c>
+      <c r="G69" t="s">
+        <v>81</v>
+      </c>
+      <c r="H69" t="s">
+        <v>366</v>
+      </c>
+      <c r="I69" t="s">
+        <v>187</v>
+      </c>
+      <c r="J69" s="2">
+        <v>14.99</v>
+      </c>
+      <c r="K69">
+        <v>2340</v>
+      </c>
+      <c r="L69">
+        <v>131322</v>
+      </c>
+      <c r="M69" t="s">
+        <v>367</v>
+      </c>
+      <c r="N69" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>298</v>
+      </c>
+      <c r="B70" t="b">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>-19</v>
+      </c>
+      <c r="E70">
+        <v>19</v>
+      </c>
+      <c r="F70" s="1">
+        <v>45428</v>
+      </c>
+      <c r="G70" t="s">
+        <v>81</v>
+      </c>
+      <c r="H70" t="s">
+        <v>299</v>
+      </c>
+      <c r="I70" t="s">
+        <v>217</v>
+      </c>
+      <c r="J70" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="K70">
+        <v>1792</v>
+      </c>
+      <c r="L70">
+        <v>26196</v>
+      </c>
+      <c r="M70" t="s">
+        <v>300</v>
+      </c>
+      <c r="N70" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>339</v>
+      </c>
+      <c r="B71" t="b">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>-12</v>
+      </c>
+      <c r="E71">
+        <v>9</v>
+      </c>
+      <c r="F71" s="1">
+        <v>45222</v>
+      </c>
+      <c r="G71" t="s">
+        <v>340</v>
+      </c>
+      <c r="H71" t="s">
+        <v>341</v>
+      </c>
+      <c r="I71" t="s">
+        <v>341</v>
+      </c>
+      <c r="J71" s="2">
+        <v>9.99</v>
+      </c>
+      <c r="K71">
+        <v>8694</v>
+      </c>
+      <c r="L71">
+        <v>345763</v>
+      </c>
+      <c r="M71" t="s">
+        <v>342</v>
+      </c>
+      <c r="N71" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>258</v>
+      </c>
+      <c r="B72" t="b">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>5</v>
+      </c>
+      <c r="E72">
+        <v>184</v>
+      </c>
+      <c r="F72" s="1">
+        <v>42879</v>
+      </c>
+      <c r="G72" t="s">
+        <v>259</v>
+      </c>
+      <c r="H72" t="s">
+        <v>260</v>
+      </c>
+      <c r="I72" t="s">
+        <v>260</v>
+      </c>
+      <c r="J72" s="2">
+        <v>9.99</v>
+      </c>
+      <c r="K72">
+        <v>364</v>
+      </c>
+      <c r="L72">
+        <v>56104</v>
+      </c>
+      <c r="M72" t="s">
+        <v>261</v>
+      </c>
+      <c r="N72" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>382</v>
+      </c>
+      <c r="B73" t="b">
+        <v>0</v>
+      </c>
+      <c r="D73" t="s">
+        <v>117</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73" s="1">
+        <v>44280</v>
+      </c>
+      <c r="G73" t="s">
+        <v>81</v>
+      </c>
+      <c r="H73" t="s">
+        <v>383</v>
+      </c>
+      <c r="I73" t="s">
+        <v>44</v>
+      </c>
+      <c r="J73" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="K73">
+        <v>2359</v>
+      </c>
+      <c r="L73">
+        <v>148861</v>
+      </c>
+      <c r="M73" t="s">
+        <v>384</v>
+      </c>
+      <c r="N73" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B74" t="b">
+        <v>0</v>
+      </c>
+      <c r="D74" t="s">
+        <v>117</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74" s="1">
+        <v>44621</v>
+      </c>
+      <c r="G74" t="s">
+        <v>315</v>
+      </c>
+      <c r="H74" t="s">
+        <v>1096</v>
+      </c>
+      <c r="I74" t="s">
+        <v>1097</v>
+      </c>
+      <c r="J74" s="2">
+        <v>14.99</v>
+      </c>
+      <c r="K74">
+        <v>238</v>
+      </c>
+      <c r="L74">
+        <v>4831</v>
+      </c>
+      <c r="N74" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B75" t="b">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>-34</v>
+      </c>
+      <c r="E75">
+        <v>3</v>
+      </c>
+      <c r="F75" s="1">
+        <v>45552</v>
+      </c>
+      <c r="G75" t="s">
+        <v>37</v>
+      </c>
+      <c r="H75" t="s">
+        <v>157</v>
+      </c>
+      <c r="I75" t="s">
+        <v>157</v>
+      </c>
+      <c r="J75" s="2">
+        <v>49.99</v>
+      </c>
+      <c r="M75" t="s">
+        <v>1167</v>
+      </c>
+      <c r="N75" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B76" t="b">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>-7</v>
+      </c>
+      <c r="E76">
+        <v>3</v>
+      </c>
+      <c r="F76" s="1">
+        <v>45575</v>
+      </c>
+      <c r="G76" t="s">
+        <v>123</v>
+      </c>
+      <c r="H76" t="s">
+        <v>1170</v>
+      </c>
+      <c r="I76" t="s">
+        <v>568</v>
+      </c>
+      <c r="J76" s="2">
+        <v>69.989999999999995</v>
+      </c>
+      <c r="M76" t="s">
+        <v>1171</v>
+      </c>
+      <c r="N76" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>531</v>
+      </c>
+      <c r="B77" t="b">
+        <v>0</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1217</v>
+      </c>
+      <c r="D77" t="s">
+        <v>117</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77" s="1">
+        <v>45267</v>
+      </c>
+      <c r="G77" t="s">
+        <v>532</v>
+      </c>
+      <c r="H77" t="s">
+        <v>533</v>
+      </c>
+      <c r="I77" t="s">
+        <v>533</v>
+      </c>
+      <c r="J77" s="2">
+        <v>49.99</v>
+      </c>
+      <c r="K77">
+        <v>452</v>
+      </c>
+      <c r="L77">
+        <v>13226</v>
+      </c>
+      <c r="M77" t="s">
+        <v>534</v>
+      </c>
+      <c r="N77" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B78" t="b">
+        <v>0</v>
+      </c>
+      <c r="D78" t="s">
+        <v>48</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78" s="1">
+        <v>45533</v>
+      </c>
+      <c r="G78" t="s">
+        <v>841</v>
+      </c>
+      <c r="H78" t="s">
+        <v>1174</v>
+      </c>
+      <c r="I78" t="s">
+        <v>1174</v>
+      </c>
+      <c r="J78" s="2">
+        <v>24.99</v>
+      </c>
+      <c r="K78">
+        <v>441</v>
+      </c>
+      <c r="M78" t="s">
+        <v>1175</v>
+      </c>
+      <c r="N78" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>620</v>
+      </c>
+      <c r="B79" t="b">
+        <v>1</v>
+      </c>
+      <c r="D79" t="s">
+        <v>117</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79" s="1">
+        <v>43054</v>
+      </c>
+      <c r="G79" t="s">
+        <v>710</v>
+      </c>
+      <c r="H79" t="s">
+        <v>621</v>
+      </c>
+      <c r="I79" t="s">
+        <v>621</v>
+      </c>
+      <c r="J79" t="s">
+        <v>27</v>
+      </c>
+      <c r="K79">
+        <v>1188</v>
+      </c>
+      <c r="L79">
+        <v>142114</v>
+      </c>
+      <c r="M79" t="s">
+        <v>622</v>
+      </c>
+      <c r="N79" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>143</v>
+      </c>
+      <c r="B80" t="b">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>-12</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+      <c r="F80" s="1">
+        <v>45284</v>
+      </c>
+      <c r="G80" t="s">
+        <v>87</v>
+      </c>
+      <c r="H80" t="s">
+        <v>144</v>
+      </c>
+      <c r="I80" t="s">
+        <v>144</v>
+      </c>
+      <c r="J80" t="s">
+        <v>27</v>
+      </c>
+      <c r="K80">
+        <v>623</v>
+      </c>
+      <c r="L80">
+        <v>5255</v>
+      </c>
+      <c r="M80" t="s">
+        <v>145</v>
+      </c>
+      <c r="N80" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>997</v>
+      </c>
+      <c r="B81" t="b">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>-23</v>
+      </c>
+      <c r="E81">
+        <v>4</v>
+      </c>
+      <c r="F81" s="1">
+        <v>44784</v>
+      </c>
+      <c r="G81" t="s">
+        <v>998</v>
+      </c>
+      <c r="H81" t="s">
+        <v>999</v>
+      </c>
+      <c r="I81" t="s">
+        <v>317</v>
+      </c>
+      <c r="J81" s="2">
+        <v>24.99</v>
+      </c>
+      <c r="K81">
+        <v>4839</v>
+      </c>
+      <c r="L81">
+        <v>74490</v>
+      </c>
+      <c r="M81" t="s">
+        <v>1000</v>
+      </c>
+      <c r="N81" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B82" t="b">
+        <v>0</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D82" t="s">
+        <v>48</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82" s="1">
+        <v>45538</v>
+      </c>
+      <c r="G82" t="s">
+        <v>572</v>
+      </c>
+      <c r="H82" t="s">
+        <v>1178</v>
+      </c>
+      <c r="I82" t="s">
+        <v>148</v>
+      </c>
+      <c r="J82" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="M82" t="s">
+        <v>1179</v>
+      </c>
+      <c r="N82" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B83" t="b">
+        <v>0</v>
+      </c>
+      <c r="D83" t="s">
+        <v>117</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83" s="1">
+        <v>44448</v>
+      </c>
+      <c r="G83" t="s">
+        <v>37</v>
+      </c>
+      <c r="H83" t="s">
+        <v>567</v>
+      </c>
+      <c r="I83" t="s">
+        <v>568</v>
+      </c>
+      <c r="J83" s="2">
+        <v>79.989999999999995</v>
+      </c>
+      <c r="K83">
+        <v>182</v>
+      </c>
+      <c r="L83">
+        <v>24966</v>
+      </c>
+      <c r="M83" t="s">
+        <v>1182</v>
+      </c>
+      <c r="N83" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>630</v>
+      </c>
+      <c r="B84" t="b">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>-2</v>
+      </c>
+      <c r="E84">
+        <v>7</v>
+      </c>
+      <c r="F84" s="1">
+        <v>40897</v>
+      </c>
+      <c r="G84" t="s">
+        <v>876</v>
+      </c>
+      <c r="H84" t="s">
+        <v>632</v>
+      </c>
+      <c r="I84" t="s">
+        <v>44</v>
+      </c>
+      <c r="J84" t="s">
+        <v>27</v>
+      </c>
+      <c r="K84">
+        <v>588</v>
+      </c>
+      <c r="L84">
+        <v>62590</v>
+      </c>
+      <c r="M84" t="s">
+        <v>633</v>
+      </c>
+      <c r="N84" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>271</v>
+      </c>
+      <c r="B85" t="b">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>16</v>
+      </c>
+      <c r="F85" s="1">
+        <v>42402</v>
+      </c>
+      <c r="G85" t="s">
+        <v>164</v>
+      </c>
+      <c r="H85" t="s">
+        <v>165</v>
+      </c>
+      <c r="I85" t="s">
+        <v>165</v>
+      </c>
+      <c r="J85" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="K85">
+        <v>1467</v>
+      </c>
+      <c r="L85">
+        <v>129990</v>
+      </c>
+      <c r="M85" t="s">
+        <v>272</v>
+      </c>
+      <c r="N85" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>402</v>
+      </c>
+      <c r="B86" t="b">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>4</v>
+      </c>
+      <c r="E86">
+        <v>3</v>
+      </c>
+      <c r="F86" s="1">
+        <v>44060</v>
+      </c>
+      <c r="G86" t="s">
+        <v>403</v>
+      </c>
+      <c r="H86" t="s">
+        <v>404</v>
+      </c>
+      <c r="I86" t="s">
+        <v>103</v>
+      </c>
+      <c r="J86" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="K86">
+        <v>658</v>
+      </c>
+      <c r="L86">
+        <v>58117</v>
+      </c>
+      <c r="M86" t="s">
+        <v>405</v>
+      </c>
+      <c r="N86" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B87" t="b">
+        <v>1</v>
+      </c>
+      <c r="D87" t="s">
+        <v>117</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="F87" s="1">
+        <v>45376</v>
+      </c>
+      <c r="G87" t="s">
+        <v>1185</v>
+      </c>
+      <c r="H87" t="s">
+        <v>1186</v>
+      </c>
+      <c r="I87" t="s">
+        <v>1186</v>
+      </c>
+      <c r="J87" t="s">
+        <v>27</v>
+      </c>
+      <c r="K87">
+        <v>1758</v>
+      </c>
+      <c r="L87">
+        <v>14422</v>
+      </c>
+      <c r="M87" t="s">
+        <v>1187</v>
+      </c>
+      <c r="N87" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B88" t="b">
+        <v>1</v>
+      </c>
+      <c r="D88">
+        <v>-68</v>
+      </c>
+      <c r="E88">
+        <v>2</v>
+      </c>
+      <c r="N88" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <v>-59</v>
+      </c>
+      <c r="E89">
+        <v>3</v>
+      </c>
+      <c r="F89" s="1">
+        <v>45519</v>
+      </c>
+      <c r="G89" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H89" t="s">
+        <v>1004</v>
+      </c>
+      <c r="I89" t="s">
+        <v>1004</v>
+      </c>
+      <c r="J89" s="2">
+        <v>24.99</v>
+      </c>
+      <c r="K89">
+        <v>5905</v>
+      </c>
+      <c r="M89" t="s">
+        <v>1005</v>
+      </c>
+      <c r="N89" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>320</v>
+      </c>
+      <c r="B90" t="b">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>-7</v>
+      </c>
+      <c r="E90">
+        <v>25</v>
+      </c>
+      <c r="F90" s="1">
+        <v>43390</v>
+      </c>
+      <c r="G90" t="s">
+        <v>321</v>
+      </c>
+      <c r="H90" t="s">
+        <v>322</v>
+      </c>
+      <c r="I90" t="s">
+        <v>322</v>
+      </c>
+      <c r="J90" s="2">
+        <v>34.99</v>
+      </c>
+      <c r="K90">
+        <v>1613</v>
+      </c>
+      <c r="L90">
+        <v>163121</v>
+      </c>
+      <c r="M90" t="s">
+        <v>323</v>
+      </c>
+      <c r="N90" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>128</v>
+      </c>
+      <c r="B91" t="b">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>-18</v>
+      </c>
+      <c r="E91">
+        <v>44</v>
+      </c>
+      <c r="F91" s="1">
+        <v>42426</v>
+      </c>
+      <c r="G91" t="s">
+        <v>129</v>
+      </c>
+      <c r="H91" t="s">
+        <v>130</v>
+      </c>
+      <c r="I91" t="s">
+        <v>130</v>
+      </c>
+      <c r="J91" s="2">
+        <v>14.99</v>
+      </c>
+      <c r="K91">
+        <v>10714</v>
+      </c>
+      <c r="L91">
+        <v>639387</v>
+      </c>
+      <c r="M91" t="s">
+        <v>131</v>
+      </c>
+      <c r="N91" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>267</v>
+      </c>
+      <c r="B92" t="b">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>-26</v>
+      </c>
+      <c r="E92">
+        <v>25</v>
+      </c>
+      <c r="F92" s="1">
+        <v>43985</v>
+      </c>
+      <c r="G92" t="s">
+        <v>81</v>
+      </c>
+      <c r="H92" t="s">
+        <v>268</v>
+      </c>
+      <c r="I92" t="s">
+        <v>103</v>
+      </c>
+      <c r="J92" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="K92">
+        <v>2665</v>
+      </c>
+      <c r="L92">
+        <v>292164</v>
+      </c>
+      <c r="M92" t="s">
+        <v>269</v>
+      </c>
+      <c r="N92" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B93" t="b">
+        <v>1</v>
+      </c>
+      <c r="D93" t="s">
+        <v>117</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+      <c r="F93" s="1">
+        <v>45028</v>
+      </c>
+      <c r="G93" t="s">
+        <v>532</v>
+      </c>
+      <c r="H93" t="s">
+        <v>1190</v>
+      </c>
+      <c r="I93" t="s">
+        <v>1190</v>
+      </c>
+      <c r="J93" s="2">
+        <v>34.99</v>
+      </c>
+      <c r="K93">
+        <v>413</v>
+      </c>
+      <c r="L93">
+        <v>23267</v>
+      </c>
+      <c r="M93" t="s">
+        <v>1191</v>
+      </c>
+      <c r="N93" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>293</v>
+      </c>
+      <c r="B94" t="b">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>-13</v>
+      </c>
+      <c r="E94">
+        <v>9</v>
+      </c>
+      <c r="F94" s="1">
+        <v>44092</v>
+      </c>
+      <c r="G94" t="s">
+        <v>294</v>
+      </c>
+      <c r="H94" t="s">
+        <v>295</v>
+      </c>
+      <c r="I94" t="s">
+        <v>295</v>
+      </c>
+      <c r="J94" s="2">
+        <v>13.99</v>
+      </c>
+      <c r="K94">
+        <v>8678</v>
+      </c>
+      <c r="L94">
+        <v>573973</v>
+      </c>
+      <c r="M94" t="s">
+        <v>296</v>
+      </c>
+      <c r="N94" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B95" t="b">
+        <v>1</v>
+      </c>
+      <c r="D95" t="s">
+        <v>48</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+      <c r="F95" s="1">
+        <v>45533</v>
+      </c>
+      <c r="G95" t="s">
+        <v>649</v>
+      </c>
+      <c r="H95" t="s">
+        <v>1132</v>
+      </c>
+      <c r="J95" s="2">
+        <v>10.99</v>
+      </c>
+      <c r="K95">
+        <v>38</v>
+      </c>
+      <c r="N95" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B96" t="b">
+        <v>0</v>
+      </c>
+      <c r="D96" t="s">
+        <v>48</v>
+      </c>
+      <c r="E96">
+        <v>1</v>
+      </c>
+      <c r="N96" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>624</v>
+      </c>
+      <c r="B97" t="b">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>2</v>
+      </c>
+      <c r="E97">
+        <v>2</v>
+      </c>
+      <c r="N97" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>949</v>
+      </c>
+      <c r="B98" t="b">
+        <v>0</v>
+      </c>
+      <c r="D98" t="s">
+        <v>117</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+      <c r="F98" s="1">
+        <v>44735</v>
+      </c>
+      <c r="G98" t="s">
+        <v>87</v>
+      </c>
+      <c r="H98" t="s">
+        <v>896</v>
+      </c>
+      <c r="I98" t="s">
+        <v>198</v>
+      </c>
+      <c r="J98" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="K98">
+        <v>471</v>
+      </c>
+      <c r="L98">
+        <v>13547</v>
+      </c>
+      <c r="M98" t="s">
+        <v>950</v>
+      </c>
+      <c r="N98" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B99" t="b">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>-24</v>
+      </c>
+      <c r="E99">
+        <v>2</v>
+      </c>
+      <c r="F99" s="1">
+        <v>42030</v>
+      </c>
+      <c r="G99" t="s">
+        <v>37</v>
+      </c>
+      <c r="H99" t="s">
+        <v>336</v>
+      </c>
+      <c r="I99" t="s">
+        <v>336</v>
+      </c>
+      <c r="J99" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="K99">
+        <v>3958</v>
+      </c>
+      <c r="L99">
+        <v>313216</v>
+      </c>
+      <c r="M99" t="s">
+        <v>1198</v>
+      </c>
+      <c r="N99" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B100" t="b">
+        <v>0</v>
+      </c>
+      <c r="D100" t="s">
+        <v>48</v>
+      </c>
+      <c r="E100">
+        <v>1</v>
+      </c>
+      <c r="F100" s="1">
+        <v>45538</v>
+      </c>
+      <c r="G100" t="s">
+        <v>1201</v>
+      </c>
+      <c r="H100" t="s">
+        <v>1202</v>
+      </c>
+      <c r="I100" t="s">
+        <v>170</v>
+      </c>
+      <c r="J100" s="2">
+        <v>29.99</v>
+      </c>
+      <c r="K100">
+        <v>99</v>
+      </c>
+      <c r="M100" t="s">
+        <v>1203</v>
+      </c>
+      <c r="N100" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B101" t="b">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>-59</v>
+      </c>
+      <c r="E101">
+        <v>2</v>
+      </c>
+      <c r="F101" s="1">
+        <v>45265</v>
+      </c>
+      <c r="G101" t="s">
+        <v>1206</v>
+      </c>
+      <c r="H101" t="s">
+        <v>1207</v>
+      </c>
+      <c r="I101" t="s">
+        <v>1207</v>
+      </c>
+      <c r="J101" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="K101">
+        <v>283</v>
+      </c>
+      <c r="L101">
+        <v>15516</v>
+      </c>
+      <c r="M101" t="s">
+        <v>1208</v>
+      </c>
+      <c r="N101" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46066FE5-CE78-B74D-B1C9-59CCDB493089}">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -7453,7 +11768,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A4B528-2005-7D49-ACA5-17BB65A55775}">
   <dimension ref="A1:L101"/>
   <sheetViews>
@@ -11222,7 +15537,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9468E3C7-ED89-7F49-91F9-C709353B7C6C}">
   <dimension ref="A1:L101"/>
   <sheetViews>
@@ -14946,7 +19261,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2439C52B-5341-DF43-8CDD-AB33FEF4C9FE}">
   <dimension ref="A1:L101"/>
   <sheetViews>
@@ -18677,7 +22992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71D7B06-37EF-F943-8D0E-B48A8AB57D51}">
   <dimension ref="A1:L101"/>
   <sheetViews>
@@ -22383,7 +26698,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3978525E-3F5E-9048-BC93-38E6C42116E5}">
   <dimension ref="A1:L101"/>
   <sheetViews>
@@ -26179,7 +30494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC291C4-96D0-D14C-9991-8EE742F649AB}">
   <dimension ref="A1:L101"/>
   <sheetViews>
@@ -29966,7 +34281,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD458E3F-9E53-804A-9E7D-8111A280BFC8}">
   <dimension ref="A1:L101"/>
   <sheetViews>

</xml_diff>